<commit_message>
Travelling Salesman Problem - check
</commit_message>
<xml_diff>
--- a/log/basline/all.xlsx
+++ b/log/basline/all.xlsx
@@ -16,94 +16,94 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
+    <t>run_1</t>
+  </si>
+  <si>
+    <t>run_10</t>
+  </si>
+  <si>
+    <t>run_11</t>
+  </si>
+  <si>
+    <t>run_12</t>
+  </si>
+  <si>
+    <t>run_13</t>
+  </si>
+  <si>
+    <t>run_14</t>
+  </si>
+  <si>
+    <t>run_15</t>
+  </si>
+  <si>
+    <t>run_16</t>
+  </si>
+  <si>
+    <t>run_17</t>
+  </si>
+  <si>
+    <t>run_18</t>
+  </si>
+  <si>
+    <t>run_19</t>
+  </si>
+  <si>
+    <t>run_2</t>
+  </si>
+  <si>
+    <t>run_20</t>
+  </si>
+  <si>
+    <t>run_21</t>
+  </si>
+  <si>
+    <t>run_22</t>
+  </si>
+  <si>
+    <t>run_23</t>
+  </si>
+  <si>
+    <t>run_24</t>
+  </si>
+  <si>
+    <t>run_25</t>
+  </si>
+  <si>
+    <t>run_26</t>
+  </si>
+  <si>
+    <t>run_27</t>
+  </si>
+  <si>
+    <t>run_28</t>
+  </si>
+  <si>
+    <t>run_29</t>
+  </si>
+  <si>
+    <t>run_3</t>
+  </si>
+  <si>
+    <t>run_30</t>
+  </si>
+  <si>
+    <t>run_4</t>
+  </si>
+  <si>
+    <t>run_5</t>
+  </si>
+  <si>
     <t>run_6</t>
   </si>
   <si>
     <t>run_7</t>
   </si>
   <si>
-    <t>run_14</t>
-  </si>
-  <si>
-    <t>run_26</t>
-  </si>
-  <si>
-    <t>run_28</t>
-  </si>
-  <si>
-    <t>run_15</t>
-  </si>
-  <si>
-    <t>run_1</t>
-  </si>
-  <si>
-    <t>run_22</t>
-  </si>
-  <si>
-    <t>run_12</t>
-  </si>
-  <si>
-    <t>run_18</t>
-  </si>
-  <si>
-    <t>run_19</t>
-  </si>
-  <si>
-    <t>run_27</t>
-  </si>
-  <si>
-    <t>run_3</t>
-  </si>
-  <si>
-    <t>run_2</t>
-  </si>
-  <si>
-    <t>run_13</t>
-  </si>
-  <si>
-    <t>run_23</t>
-  </si>
-  <si>
-    <t>run_11</t>
-  </si>
-  <si>
-    <t>run_24</t>
-  </si>
-  <si>
-    <t>run_17</t>
-  </si>
-  <si>
     <t>run_8</t>
   </si>
   <si>
-    <t>run_5</t>
-  </si>
-  <si>
-    <t>run_20</t>
-  </si>
-  <si>
-    <t>run_29</t>
-  </si>
-  <si>
-    <t>run_25</t>
-  </si>
-  <si>
     <t>run_9</t>
-  </si>
-  <si>
-    <t>run_4</t>
-  </si>
-  <si>
-    <t>run_30</t>
-  </si>
-  <si>
-    <t>run_10</t>
-  </si>
-  <si>
-    <t>run_16</t>
-  </si>
-  <si>
-    <t>run_21</t>
   </si>
   <si>
     <t>Generation</t>
@@ -591,1500 +591,1500 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2">
-        <v>4149</v>
+        <v>4168</v>
       </c>
       <c r="B2">
-        <v>4356</v>
+        <v>3300</v>
       </c>
       <c r="C2">
-        <v>3890</v>
+        <v>3521</v>
       </c>
       <c r="D2">
-        <v>4197</v>
+        <v>3923</v>
       </c>
       <c r="E2">
-        <v>3290</v>
+        <v>4071</v>
       </c>
       <c r="F2">
-        <v>3574</v>
+        <v>2901</v>
       </c>
       <c r="G2">
-        <v>4349</v>
+        <v>3179</v>
       </c>
       <c r="H2">
-        <v>3425</v>
+        <v>3550</v>
       </c>
       <c r="I2">
-        <v>3988</v>
+        <v>4016</v>
       </c>
       <c r="J2">
-        <v>3613</v>
+        <v>4652</v>
       </c>
       <c r="K2">
-        <v>3498</v>
+        <v>3710</v>
       </c>
       <c r="L2">
-        <v>3861</v>
+        <v>3461</v>
       </c>
       <c r="M2">
-        <v>3880</v>
+        <v>4030</v>
       </c>
       <c r="N2">
-        <v>3868</v>
+        <v>4186</v>
       </c>
       <c r="O2">
-        <v>4274</v>
+        <v>3482</v>
       </c>
       <c r="P2">
-        <v>4424</v>
+        <v>4014</v>
       </c>
       <c r="Q2">
-        <v>3936</v>
+        <v>3798</v>
       </c>
       <c r="R2">
-        <v>3545</v>
+        <v>4264</v>
       </c>
       <c r="S2">
-        <v>3688</v>
+        <v>3660</v>
       </c>
       <c r="T2">
-        <v>3908</v>
+        <v>4617</v>
       </c>
       <c r="U2">
-        <v>3364</v>
+        <v>3592</v>
       </c>
       <c r="V2">
-        <v>4008</v>
+        <v>3325</v>
       </c>
       <c r="W2">
-        <v>3529</v>
+        <v>4101</v>
       </c>
       <c r="X2">
-        <v>4434</v>
+        <v>3774</v>
       </c>
       <c r="Y2">
-        <v>4054</v>
+        <v>3770</v>
       </c>
       <c r="Z2">
-        <v>4274</v>
+        <v>3833</v>
       </c>
       <c r="AA2">
-        <v>3627</v>
+        <v>3883</v>
       </c>
       <c r="AB2">
-        <v>3900</v>
+        <v>3683</v>
       </c>
       <c r="AC2">
-        <v>3976</v>
+        <v>4493</v>
       </c>
       <c r="AD2">
-        <v>3674</v>
+        <v>3852</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>327.7594102912726</v>
+        <v>406.7886414965082</v>
       </c>
       <c r="AG2">
-        <v>3885.1</v>
+        <v>3826.966666666667</v>
       </c>
       <c r="AH2">
-        <v>4212.859410291272</v>
+        <v>4233.755308163175</v>
       </c>
       <c r="AI2">
-        <v>3557.340589708727</v>
+        <v>3420.178025170158</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3">
-        <v>4158</v>
+        <v>4332</v>
       </c>
       <c r="B3">
-        <v>4668</v>
+        <v>3583</v>
       </c>
       <c r="C3">
-        <v>3890</v>
+        <v>4201</v>
       </c>
       <c r="D3">
-        <v>4197</v>
+        <v>4028</v>
       </c>
       <c r="E3">
-        <v>3758</v>
+        <v>4251</v>
       </c>
       <c r="F3">
-        <v>3658</v>
+        <v>3591</v>
       </c>
       <c r="G3">
-        <v>4388</v>
+        <v>3701</v>
       </c>
       <c r="H3">
-        <v>3711</v>
+        <v>4360</v>
       </c>
       <c r="I3">
-        <v>4620</v>
+        <v>4199</v>
       </c>
       <c r="J3">
-        <v>3881</v>
+        <v>4652</v>
       </c>
       <c r="K3">
-        <v>4165</v>
+        <v>4022</v>
       </c>
       <c r="L3">
-        <v>3944</v>
+        <v>3719</v>
       </c>
       <c r="M3">
-        <v>4260</v>
+        <v>4030</v>
       </c>
       <c r="N3">
-        <v>3892</v>
+        <v>4727</v>
       </c>
       <c r="O3">
-        <v>4416</v>
+        <v>4269</v>
       </c>
       <c r="P3">
-        <v>4438</v>
+        <v>4291</v>
       </c>
       <c r="Q3">
-        <v>4320</v>
+        <v>4124</v>
       </c>
       <c r="R3">
-        <v>3548</v>
+        <v>4676</v>
       </c>
       <c r="S3">
-        <v>4189</v>
+        <v>3833</v>
       </c>
       <c r="T3">
-        <v>4001</v>
+        <v>4685</v>
       </c>
       <c r="U3">
-        <v>3562</v>
+        <v>3804</v>
       </c>
       <c r="V3">
-        <v>4008</v>
+        <v>4090</v>
       </c>
       <c r="W3">
-        <v>3845</v>
+        <v>4544</v>
       </c>
       <c r="X3">
-        <v>4686</v>
+        <v>3989</v>
       </c>
       <c r="Y3">
-        <v>4196</v>
+        <v>4685</v>
       </c>
       <c r="Z3">
-        <v>4471</v>
+        <v>3833</v>
       </c>
       <c r="AA3">
-        <v>3746</v>
+        <v>4091</v>
       </c>
       <c r="AB3">
-        <v>4172</v>
+        <v>3867</v>
       </c>
       <c r="AC3">
-        <v>4353</v>
+        <v>4558</v>
       </c>
       <c r="AD3">
-        <v>3674</v>
+        <v>4145</v>
       </c>
       <c r="AE3">
         <v>1</v>
       </c>
       <c r="AF3">
-        <v>329.8292226167264</v>
+        <v>341.3412018669209</v>
       </c>
       <c r="AG3">
-        <v>4093.833333333333</v>
+        <v>4162.666666666667</v>
       </c>
       <c r="AH3">
-        <v>4423.66255595006</v>
+        <v>4504.007868533587</v>
       </c>
       <c r="AI3">
-        <v>3764.004110716607</v>
+        <v>3821.325464799746</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4">
-        <v>4680</v>
+        <v>4332</v>
       </c>
       <c r="B4">
-        <v>4668</v>
+        <v>3785</v>
       </c>
       <c r="C4">
-        <v>3932</v>
+        <v>4272</v>
       </c>
       <c r="D4">
-        <v>4197</v>
+        <v>4312</v>
       </c>
       <c r="E4">
-        <v>3969</v>
+        <v>4372</v>
       </c>
       <c r="F4">
-        <v>3804</v>
+        <v>4028</v>
       </c>
       <c r="G4">
-        <v>5019</v>
+        <v>3937</v>
       </c>
       <c r="H4">
-        <v>4187</v>
+        <v>4729</v>
       </c>
       <c r="I4">
-        <v>4733</v>
+        <v>4429</v>
       </c>
       <c r="J4">
-        <v>4010</v>
+        <v>4664</v>
       </c>
       <c r="K4">
-        <v>4165</v>
+        <v>4481</v>
       </c>
       <c r="L4">
-        <v>3961</v>
+        <v>3719</v>
       </c>
       <c r="M4">
-        <v>4490</v>
+        <v>4030</v>
       </c>
       <c r="N4">
-        <v>4413</v>
+        <v>4810</v>
       </c>
       <c r="O4">
-        <v>4416</v>
+        <v>4293</v>
       </c>
       <c r="P4">
-        <v>4944</v>
+        <v>4603</v>
       </c>
       <c r="Q4">
-        <v>4803</v>
+        <v>4584</v>
       </c>
       <c r="R4">
-        <v>3787</v>
+        <v>4769</v>
       </c>
       <c r="S4">
-        <v>4226</v>
+        <v>4203</v>
       </c>
       <c r="T4">
-        <v>4029</v>
+        <v>5060</v>
       </c>
       <c r="U4">
-        <v>3916</v>
+        <v>4036</v>
       </c>
       <c r="V4">
-        <v>4089</v>
+        <v>4289</v>
       </c>
       <c r="W4">
-        <v>3984</v>
+        <v>4544</v>
       </c>
       <c r="X4">
-        <v>4686</v>
+        <v>4136</v>
       </c>
       <c r="Y4">
-        <v>4651</v>
+        <v>4685</v>
       </c>
       <c r="Z4">
-        <v>4471</v>
+        <v>3869</v>
       </c>
       <c r="AA4">
-        <v>4036</v>
+        <v>4091</v>
       </c>
       <c r="AB4">
-        <v>4440</v>
+        <v>4258</v>
       </c>
       <c r="AC4">
-        <v>4353</v>
+        <v>4782</v>
       </c>
       <c r="AD4">
-        <v>3758</v>
+        <v>4145</v>
       </c>
       <c r="AE4">
         <v>2</v>
       </c>
       <c r="AF4">
-        <v>360.367566185722</v>
+        <v>333.9571192103327</v>
       </c>
       <c r="AG4">
-        <v>4293.9</v>
+        <v>4341.566666666667</v>
       </c>
       <c r="AH4">
-        <v>4654.267566185722</v>
+        <v>4675.523785877</v>
       </c>
       <c r="AI4">
-        <v>3933.532433814278</v>
+        <v>4007.609547456334</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5">
-        <v>4680</v>
+        <v>4749</v>
       </c>
       <c r="B5">
-        <v>4668</v>
+        <v>4240</v>
       </c>
       <c r="C5">
-        <v>4147</v>
+        <v>4331</v>
       </c>
       <c r="D5">
-        <v>4197</v>
+        <v>4312</v>
       </c>
       <c r="E5">
+        <v>4603</v>
+      </c>
+      <c r="F5">
+        <v>4338</v>
+      </c>
+      <c r="G5">
+        <v>4073</v>
+      </c>
+      <c r="H5">
+        <v>4729</v>
+      </c>
+      <c r="I5">
+        <v>4787</v>
+      </c>
+      <c r="J5">
+        <v>4706</v>
+      </c>
+      <c r="K5">
+        <v>4540</v>
+      </c>
+      <c r="L5">
+        <v>4195</v>
+      </c>
+      <c r="M5">
+        <v>4390</v>
+      </c>
+      <c r="N5">
+        <v>5039</v>
+      </c>
+      <c r="O5">
+        <v>5095</v>
+      </c>
+      <c r="P5">
+        <v>4686</v>
+      </c>
+      <c r="Q5">
+        <v>4626</v>
+      </c>
+      <c r="R5">
+        <v>4769</v>
+      </c>
+      <c r="S5">
+        <v>4203</v>
+      </c>
+      <c r="T5">
+        <v>5060</v>
+      </c>
+      <c r="U5">
+        <v>4161</v>
+      </c>
+      <c r="V5">
+        <v>4410</v>
+      </c>
+      <c r="W5">
+        <v>4544</v>
+      </c>
+      <c r="X5">
         <v>4136</v>
       </c>
-      <c r="F5">
-        <v>3970</v>
-      </c>
-      <c r="G5">
-        <v>5019</v>
-      </c>
-      <c r="H5">
-        <v>4435</v>
-      </c>
-      <c r="I5">
-        <v>4769</v>
-      </c>
-      <c r="J5">
-        <v>4501</v>
-      </c>
-      <c r="K5">
-        <v>4165</v>
-      </c>
-      <c r="L5">
-        <v>3961</v>
-      </c>
-      <c r="M5">
-        <v>4537</v>
-      </c>
-      <c r="N5">
-        <v>4413</v>
-      </c>
-      <c r="O5">
-        <v>4416</v>
-      </c>
-      <c r="P5">
-        <v>4944</v>
-      </c>
-      <c r="Q5">
-        <v>5021</v>
-      </c>
-      <c r="R5">
-        <v>3941</v>
-      </c>
-      <c r="S5">
-        <v>4276</v>
-      </c>
-      <c r="T5">
-        <v>4546</v>
-      </c>
-      <c r="U5">
-        <v>3916</v>
-      </c>
-      <c r="V5">
-        <v>4389</v>
-      </c>
-      <c r="W5">
-        <v>4284</v>
-      </c>
-      <c r="X5">
-        <v>4928</v>
-      </c>
       <c r="Y5">
-        <v>4928</v>
+        <v>4699</v>
       </c>
       <c r="Z5">
-        <v>4570</v>
+        <v>3995</v>
       </c>
       <c r="AA5">
-        <v>4530</v>
+        <v>4173</v>
       </c>
       <c r="AB5">
-        <v>4731</v>
+        <v>4586</v>
       </c>
       <c r="AC5">
-        <v>4353</v>
+        <v>4872</v>
       </c>
       <c r="AD5">
-        <v>3977</v>
+        <v>4400</v>
       </c>
       <c r="AE5">
         <v>3</v>
       </c>
       <c r="AF5">
-        <v>338.2615732743271</v>
+        <v>303.6544485726021</v>
       </c>
       <c r="AG5">
-        <v>4444.933333333333</v>
+        <v>4514.9</v>
       </c>
       <c r="AH5">
-        <v>4783.19490660766</v>
+        <v>4818.554448572601</v>
       </c>
       <c r="AI5">
-        <v>4106.671760059006</v>
+        <v>4211.245551427398</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6">
-        <v>4749</v>
+        <v>5059</v>
       </c>
       <c r="B6">
-        <v>4756</v>
+        <v>4515</v>
       </c>
       <c r="C6">
-        <v>4147</v>
+        <v>4331</v>
       </c>
       <c r="D6">
-        <v>4381</v>
+        <v>4366</v>
       </c>
       <c r="E6">
-        <v>4200</v>
+        <v>4815</v>
       </c>
       <c r="F6">
-        <v>4198</v>
+        <v>4586</v>
       </c>
       <c r="G6">
-        <v>5058</v>
+        <v>4167</v>
       </c>
       <c r="H6">
-        <v>4879</v>
+        <v>4807</v>
       </c>
       <c r="I6">
-        <v>4814</v>
+        <v>5245</v>
       </c>
       <c r="J6">
-        <v>4551</v>
+        <v>4936</v>
       </c>
       <c r="K6">
-        <v>4229</v>
+        <v>4722</v>
       </c>
       <c r="L6">
-        <v>4010</v>
+        <v>4400</v>
       </c>
       <c r="M6">
-        <v>4573</v>
+        <v>4708</v>
       </c>
       <c r="N6">
-        <v>4413</v>
+        <v>5167</v>
       </c>
       <c r="O6">
-        <v>4416</v>
+        <v>5095</v>
       </c>
       <c r="P6">
-        <v>5016</v>
+        <v>4759</v>
       </c>
       <c r="Q6">
-        <v>5063</v>
+        <v>4948</v>
       </c>
       <c r="R6">
-        <v>4301</v>
+        <v>4858</v>
       </c>
       <c r="S6">
-        <v>4280</v>
+        <v>4203</v>
       </c>
       <c r="T6">
-        <v>4911</v>
+        <v>5060</v>
       </c>
       <c r="U6">
-        <v>4291</v>
+        <v>4669</v>
       </c>
       <c r="V6">
-        <v>4409</v>
+        <v>4521</v>
       </c>
       <c r="W6">
-        <v>4284</v>
+        <v>4689</v>
       </c>
       <c r="X6">
-        <v>4937</v>
+        <v>4136</v>
       </c>
       <c r="Y6">
-        <v>5016</v>
+        <v>4777</v>
       </c>
       <c r="Z6">
-        <v>4570</v>
+        <v>3997</v>
       </c>
       <c r="AA6">
-        <v>4617</v>
+        <v>4332</v>
       </c>
       <c r="AB6">
-        <v>4731</v>
+        <v>4586</v>
       </c>
       <c r="AC6">
-        <v>4353</v>
+        <v>4872</v>
       </c>
       <c r="AD6">
-        <v>4224</v>
+        <v>4660</v>
       </c>
       <c r="AE6">
         <v>4</v>
       </c>
       <c r="AF6">
-        <v>312.9243987137226</v>
+        <v>322.3411557490838</v>
       </c>
       <c r="AG6">
-        <v>4545.9</v>
+        <v>4666.2</v>
       </c>
       <c r="AH6">
-        <v>4858.824398713722</v>
+        <v>4988.541155749083</v>
       </c>
       <c r="AI6">
-        <v>4232.975601286277</v>
+        <v>4343.858844250916</v>
       </c>
     </row>
     <row r="7" spans="1:35">
       <c r="A7">
-        <v>4826</v>
+        <v>5125</v>
       </c>
       <c r="B7">
-        <v>4756</v>
+        <v>4515</v>
       </c>
       <c r="C7">
-        <v>4184</v>
+        <v>4331</v>
       </c>
       <c r="D7">
-        <v>4381</v>
+        <v>4535</v>
       </c>
       <c r="E7">
-        <v>4454</v>
+        <v>4870</v>
       </c>
       <c r="F7">
-        <v>4198</v>
+        <v>4794</v>
       </c>
       <c r="G7">
-        <v>5058</v>
+        <v>4316</v>
       </c>
       <c r="H7">
-        <v>4879</v>
+        <v>4812</v>
       </c>
       <c r="I7">
-        <v>4853</v>
+        <v>5245</v>
       </c>
       <c r="J7">
-        <v>4746</v>
+        <v>4964</v>
       </c>
       <c r="K7">
-        <v>4355</v>
+        <v>4722</v>
       </c>
       <c r="L7">
-        <v>4243</v>
+        <v>4472</v>
       </c>
       <c r="M7">
-        <v>4610</v>
+        <v>4708</v>
       </c>
       <c r="N7">
-        <v>4624</v>
+        <v>5167</v>
       </c>
       <c r="O7">
-        <v>4431</v>
+        <v>5140</v>
       </c>
       <c r="P7">
-        <v>5016</v>
+        <v>4759</v>
       </c>
       <c r="Q7">
-        <v>5126</v>
+        <v>4948</v>
       </c>
       <c r="R7">
-        <v>4396</v>
+        <v>4858</v>
       </c>
       <c r="S7">
-        <v>4493</v>
+        <v>4203</v>
       </c>
       <c r="T7">
-        <v>4911</v>
+        <v>5087</v>
       </c>
       <c r="U7">
-        <v>4314</v>
+        <v>4850</v>
       </c>
       <c r="V7">
-        <v>4451</v>
+        <v>4720</v>
       </c>
       <c r="W7">
-        <v>4821</v>
+        <v>4689</v>
       </c>
       <c r="X7">
-        <v>4937</v>
+        <v>4220</v>
       </c>
       <c r="Y7">
-        <v>5229</v>
+        <v>4777</v>
       </c>
       <c r="Z7">
-        <v>4605</v>
+        <v>4254</v>
       </c>
       <c r="AA7">
-        <v>5002</v>
+        <v>4683</v>
       </c>
       <c r="AB7">
-        <v>5060</v>
+        <v>4586</v>
       </c>
       <c r="AC7">
-        <v>4353</v>
+        <v>4929</v>
       </c>
       <c r="AD7">
-        <v>4458</v>
+        <v>4660</v>
       </c>
       <c r="AE7">
         <v>5</v>
       </c>
       <c r="AF7">
-        <v>304.0263146505578</v>
+        <v>287.068554830399</v>
       </c>
       <c r="AG7">
-        <v>4659</v>
+        <v>4731.3</v>
       </c>
       <c r="AH7">
-        <v>4963.026314650558</v>
+        <v>5018.368554830399</v>
       </c>
       <c r="AI7">
-        <v>4354.973685349442</v>
+        <v>4444.231445169601</v>
       </c>
     </row>
     <row r="8" spans="1:35">
       <c r="A8">
-        <v>4988</v>
+        <v>5125</v>
       </c>
       <c r="B8">
-        <v>4756</v>
+        <v>4671</v>
       </c>
       <c r="C8">
-        <v>4348</v>
+        <v>4374</v>
       </c>
       <c r="D8">
-        <v>4381</v>
+        <v>4535</v>
       </c>
       <c r="E8">
-        <v>4454</v>
+        <v>4870</v>
       </c>
       <c r="F8">
-        <v>4198</v>
+        <v>4794</v>
       </c>
       <c r="G8">
-        <v>5093</v>
+        <v>4326</v>
       </c>
       <c r="H8">
-        <v>4926</v>
+        <v>4890</v>
       </c>
       <c r="I8">
-        <v>5051</v>
+        <v>5245</v>
       </c>
       <c r="J8">
-        <v>4843</v>
+        <v>4976</v>
       </c>
       <c r="K8">
-        <v>4386</v>
+        <v>4805</v>
       </c>
       <c r="L8">
-        <v>4321</v>
+        <v>4528</v>
       </c>
       <c r="M8">
-        <v>4610</v>
+        <v>4708</v>
       </c>
       <c r="N8">
-        <v>4624</v>
+        <v>5294</v>
       </c>
       <c r="O8">
-        <v>4431</v>
+        <v>5173</v>
       </c>
       <c r="P8">
-        <v>5039</v>
+        <v>4759</v>
       </c>
       <c r="Q8">
-        <v>5126</v>
+        <v>4948</v>
       </c>
       <c r="R8">
-        <v>4396</v>
+        <v>5129</v>
       </c>
       <c r="S8">
-        <v>4673</v>
+        <v>4290</v>
       </c>
       <c r="T8">
-        <v>5147</v>
+        <v>5087</v>
       </c>
       <c r="U8">
-        <v>4314</v>
+        <v>4898</v>
       </c>
       <c r="V8">
-        <v>4634</v>
+        <v>5102</v>
       </c>
       <c r="W8">
-        <v>4976</v>
+        <v>4932</v>
       </c>
       <c r="X8">
-        <v>4938</v>
+        <v>4220</v>
       </c>
       <c r="Y8">
-        <v>5288</v>
+        <v>4777</v>
       </c>
       <c r="Z8">
-        <v>4638</v>
+        <v>4254</v>
       </c>
       <c r="AA8">
-        <v>5345</v>
+        <v>4733</v>
       </c>
       <c r="AB8">
-        <v>5060</v>
+        <v>4635</v>
       </c>
       <c r="AC8">
-        <v>4489</v>
+        <v>4935</v>
       </c>
       <c r="AD8">
-        <v>4458</v>
+        <v>4660</v>
       </c>
       <c r="AE8">
         <v>6</v>
       </c>
       <c r="AF8">
-        <v>329.4113331942021</v>
+        <v>299.4169449055142</v>
       </c>
       <c r="AG8">
-        <v>4731.033333333334</v>
+        <v>4789.1</v>
       </c>
       <c r="AH8">
-        <v>5060.444666527535</v>
+        <v>5088.516944905515</v>
       </c>
       <c r="AI8">
-        <v>4401.622000139132</v>
+        <v>4489.683055094486</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9">
-        <v>5188</v>
+        <v>5125</v>
       </c>
       <c r="B9">
-        <v>4770</v>
+        <v>4671</v>
       </c>
       <c r="C9">
-        <v>4421</v>
+        <v>4374</v>
       </c>
       <c r="D9">
-        <v>4381</v>
+        <v>4535</v>
       </c>
       <c r="E9">
-        <v>5014</v>
+        <v>5031</v>
       </c>
       <c r="F9">
-        <v>4270</v>
+        <v>4839</v>
       </c>
       <c r="G9">
-        <v>5093</v>
+        <v>4479</v>
       </c>
       <c r="H9">
-        <v>5037</v>
+        <v>4890</v>
       </c>
       <c r="I9">
-        <v>5062</v>
+        <v>5245</v>
       </c>
       <c r="J9">
+        <v>4976</v>
+      </c>
+      <c r="K9">
+        <v>4805</v>
+      </c>
+      <c r="L9">
+        <v>4958</v>
+      </c>
+      <c r="M9">
+        <v>4831</v>
+      </c>
+      <c r="N9">
+        <v>5294</v>
+      </c>
+      <c r="O9">
+        <v>5495</v>
+      </c>
+      <c r="P9">
+        <v>4814</v>
+      </c>
+      <c r="Q9">
+        <v>4948</v>
+      </c>
+      <c r="R9">
+        <v>5129</v>
+      </c>
+      <c r="S9">
+        <v>4290</v>
+      </c>
+      <c r="T9">
+        <v>5148</v>
+      </c>
+      <c r="U9">
+        <v>5005</v>
+      </c>
+      <c r="V9">
+        <v>5130</v>
+      </c>
+      <c r="W9">
+        <v>4932</v>
+      </c>
+      <c r="X9">
+        <v>4398</v>
+      </c>
+      <c r="Y9">
+        <v>4887</v>
+      </c>
+      <c r="Z9">
+        <v>4611</v>
+      </c>
+      <c r="AA9">
+        <v>4733</v>
+      </c>
+      <c r="AB9">
+        <v>4635</v>
+      </c>
+      <c r="AC9">
+        <v>4979</v>
+      </c>
+      <c r="AD9">
         <v>4937</v>
-      </c>
-      <c r="K9">
-        <v>4414</v>
-      </c>
-      <c r="L9">
-        <v>4422</v>
-      </c>
-      <c r="M9">
-        <v>4808</v>
-      </c>
-      <c r="N9">
-        <v>4738</v>
-      </c>
-      <c r="O9">
-        <v>4431</v>
-      </c>
-      <c r="P9">
-        <v>5076</v>
-      </c>
-      <c r="Q9">
-        <v>5399</v>
-      </c>
-      <c r="R9">
-        <v>4448</v>
-      </c>
-      <c r="S9">
-        <v>4723</v>
-      </c>
-      <c r="T9">
-        <v>5147</v>
-      </c>
-      <c r="U9">
-        <v>4319</v>
-      </c>
-      <c r="V9">
-        <v>4799</v>
-      </c>
-      <c r="W9">
-        <v>4981</v>
-      </c>
-      <c r="X9">
-        <v>5331</v>
-      </c>
-      <c r="Y9">
-        <v>5288</v>
-      </c>
-      <c r="Z9">
-        <v>4865</v>
-      </c>
-      <c r="AA9">
-        <v>5345</v>
-      </c>
-      <c r="AB9">
-        <v>5079</v>
-      </c>
-      <c r="AC9">
-        <v>4542</v>
-      </c>
-      <c r="AD9">
-        <v>4663</v>
       </c>
       <c r="AE9">
         <v>7</v>
       </c>
       <c r="AF9">
-        <v>340.377932277651</v>
+        <v>283.9945846982491</v>
       </c>
       <c r="AG9">
-        <v>4833.033333333334</v>
+        <v>4870.8</v>
       </c>
       <c r="AH9">
-        <v>5173.411265610985</v>
+        <v>5154.794584698249</v>
       </c>
       <c r="AI9">
-        <v>4492.655401055683</v>
+        <v>4586.805415301751</v>
       </c>
     </row>
     <row r="10" spans="1:35">
       <c r="A10">
-        <v>5216</v>
+        <v>5125</v>
       </c>
       <c r="B10">
-        <v>4770</v>
+        <v>4998</v>
       </c>
       <c r="C10">
-        <v>4478</v>
+        <v>4407</v>
       </c>
       <c r="D10">
-        <v>4511</v>
+        <v>4535</v>
       </c>
       <c r="E10">
-        <v>5014</v>
+        <v>5031</v>
       </c>
       <c r="F10">
-        <v>4310</v>
+        <v>4852</v>
       </c>
       <c r="G10">
-        <v>5093</v>
+        <v>4633</v>
       </c>
       <c r="H10">
-        <v>5037</v>
+        <v>4890</v>
       </c>
       <c r="I10">
-        <v>5110</v>
+        <v>5245</v>
       </c>
       <c r="J10">
-        <v>5220</v>
+        <v>4976</v>
       </c>
       <c r="K10">
-        <v>4414</v>
+        <v>4805</v>
       </c>
       <c r="L10">
-        <v>4422</v>
+        <v>5002</v>
       </c>
       <c r="M10">
-        <v>4884</v>
+        <v>5248</v>
       </c>
       <c r="N10">
-        <v>4738</v>
+        <v>5399</v>
       </c>
       <c r="O10">
-        <v>4459</v>
+        <v>5495</v>
       </c>
       <c r="P10">
-        <v>5076</v>
+        <v>4814</v>
       </c>
       <c r="Q10">
-        <v>5419</v>
+        <v>4986</v>
       </c>
       <c r="R10">
-        <v>4902</v>
+        <v>5129</v>
       </c>
       <c r="S10">
-        <v>4723</v>
+        <v>4290</v>
       </c>
       <c r="T10">
-        <v>5175</v>
+        <v>5148</v>
       </c>
       <c r="U10">
-        <v>4468</v>
+        <v>5005</v>
       </c>
       <c r="V10">
-        <v>4799</v>
+        <v>5130</v>
       </c>
       <c r="W10">
-        <v>4981</v>
+        <v>4932</v>
       </c>
       <c r="X10">
-        <v>5331</v>
+        <v>4557</v>
       </c>
       <c r="Y10">
-        <v>5288</v>
+        <v>4929</v>
       </c>
       <c r="Z10">
-        <v>4865</v>
+        <v>4983</v>
       </c>
       <c r="AA10">
-        <v>5345</v>
+        <v>4733</v>
       </c>
       <c r="AB10">
-        <v>5299</v>
+        <v>4818</v>
       </c>
       <c r="AC10">
-        <v>4678</v>
+        <v>5068</v>
       </c>
       <c r="AD10">
-        <v>4696</v>
+        <v>4937</v>
       </c>
       <c r="AE10">
         <v>8</v>
       </c>
       <c r="AF10">
-        <v>326.3792114323037</v>
+        <v>269.786292606131</v>
       </c>
       <c r="AG10">
-        <v>4890.7</v>
+        <v>4936.666666666667</v>
       </c>
       <c r="AH10">
-        <v>5217.079211432304</v>
+        <v>5206.452959272798</v>
       </c>
       <c r="AI10">
-        <v>4564.320788567696</v>
+        <v>4666.880374060536</v>
       </c>
     </row>
     <row r="11" spans="1:35">
       <c r="A11">
-        <v>5258</v>
+        <v>5125</v>
       </c>
       <c r="B11">
-        <v>4962</v>
+        <v>5031</v>
       </c>
       <c r="C11">
-        <v>4478</v>
+        <v>4407</v>
       </c>
       <c r="D11">
-        <v>4741</v>
+        <v>4535</v>
       </c>
       <c r="E11">
-        <v>5014</v>
+        <v>5109</v>
       </c>
       <c r="F11">
-        <v>4335</v>
+        <v>4852</v>
       </c>
       <c r="G11">
-        <v>5093</v>
+        <v>4694</v>
       </c>
       <c r="H11">
-        <v>5037</v>
+        <v>4890</v>
       </c>
       <c r="I11">
+        <v>5245</v>
+      </c>
+      <c r="J11">
+        <v>4976</v>
+      </c>
+      <c r="K11">
+        <v>4916</v>
+      </c>
+      <c r="L11">
+        <v>5002</v>
+      </c>
+      <c r="M11">
+        <v>5291</v>
+      </c>
+      <c r="N11">
+        <v>5399</v>
+      </c>
+      <c r="O11">
+        <v>5605</v>
+      </c>
+      <c r="P11">
+        <v>4814</v>
+      </c>
+      <c r="Q11">
+        <v>5332</v>
+      </c>
+      <c r="R11">
+        <v>5129</v>
+      </c>
+      <c r="S11">
+        <v>4294</v>
+      </c>
+      <c r="T11">
+        <v>5148</v>
+      </c>
+      <c r="U11">
+        <v>5113</v>
+      </c>
+      <c r="V11">
+        <v>5359</v>
+      </c>
+      <c r="W11">
+        <v>4932</v>
+      </c>
+      <c r="X11">
+        <v>4876</v>
+      </c>
+      <c r="Y11">
+        <v>4934</v>
+      </c>
+      <c r="Z11">
+        <v>4983</v>
+      </c>
+      <c r="AA11">
+        <v>4797</v>
+      </c>
+      <c r="AB11">
+        <v>5232</v>
+      </c>
+      <c r="AC11">
         <v>5132</v>
       </c>
-      <c r="J11">
-        <v>5235</v>
-      </c>
-      <c r="K11">
-        <v>4414</v>
-      </c>
-      <c r="L11">
-        <v>4565</v>
-      </c>
-      <c r="M11">
-        <v>4884</v>
-      </c>
-      <c r="N11">
-        <v>4788</v>
-      </c>
-      <c r="O11">
-        <v>4487</v>
-      </c>
-      <c r="P11">
-        <v>5406</v>
-      </c>
-      <c r="Q11">
-        <v>5419</v>
-      </c>
-      <c r="R11">
-        <v>4902</v>
-      </c>
-      <c r="S11">
-        <v>4803</v>
-      </c>
-      <c r="T11">
-        <v>5175</v>
-      </c>
-      <c r="U11">
-        <v>4534</v>
-      </c>
-      <c r="V11">
-        <v>4945</v>
-      </c>
-      <c r="W11">
-        <v>4981</v>
-      </c>
-      <c r="X11">
-        <v>5331</v>
-      </c>
-      <c r="Y11">
-        <v>5288</v>
-      </c>
-      <c r="Z11">
-        <v>4865</v>
-      </c>
-      <c r="AA11">
-        <v>5345</v>
-      </c>
-      <c r="AB11">
-        <v>5299</v>
-      </c>
-      <c r="AC11">
-        <v>4829</v>
-      </c>
       <c r="AD11">
-        <v>4712</v>
+        <v>4966</v>
       </c>
       <c r="AE11">
         <v>9</v>
       </c>
       <c r="AF11">
-        <v>313.8691084534751</v>
+        <v>285.4393991282784</v>
       </c>
       <c r="AG11">
-        <v>4941.9</v>
+        <v>5003.933333333333</v>
       </c>
       <c r="AH11">
-        <v>5255.769108453474</v>
+        <v>5289.372732461612</v>
       </c>
       <c r="AI11">
-        <v>4628.030891546525</v>
+        <v>4718.493934205055</v>
       </c>
     </row>
     <row r="12" spans="1:35">
       <c r="A12">
-        <v>5275</v>
+        <v>5125</v>
       </c>
       <c r="B12">
-        <v>4962</v>
+        <v>5088</v>
       </c>
       <c r="C12">
-        <v>4603</v>
+        <v>4407</v>
       </c>
       <c r="D12">
+        <v>4535</v>
+      </c>
+      <c r="E12">
+        <v>5151</v>
+      </c>
+      <c r="F12">
+        <v>4852</v>
+      </c>
+      <c r="G12">
+        <v>4694</v>
+      </c>
+      <c r="H12">
+        <v>4890</v>
+      </c>
+      <c r="I12">
+        <v>5245</v>
+      </c>
+      <c r="J12">
+        <v>4976</v>
+      </c>
+      <c r="K12">
+        <v>4972</v>
+      </c>
+      <c r="L12">
+        <v>5021</v>
+      </c>
+      <c r="M12">
+        <v>5304</v>
+      </c>
+      <c r="N12">
+        <v>5399</v>
+      </c>
+      <c r="O12">
+        <v>5605</v>
+      </c>
+      <c r="P12">
+        <v>5015</v>
+      </c>
+      <c r="Q12">
+        <v>5332</v>
+      </c>
+      <c r="R12">
+        <v>5316</v>
+      </c>
+      <c r="S12">
+        <v>4332</v>
+      </c>
+      <c r="T12">
+        <v>5148</v>
+      </c>
+      <c r="U12">
+        <v>5113</v>
+      </c>
+      <c r="V12">
+        <v>5359</v>
+      </c>
+      <c r="W12">
+        <v>4932</v>
+      </c>
+      <c r="X12">
+        <v>4912</v>
+      </c>
+      <c r="Y12">
+        <v>4989</v>
+      </c>
+      <c r="Z12">
+        <v>4983</v>
+      </c>
+      <c r="AA12">
+        <v>4797</v>
+      </c>
+      <c r="AB12">
+        <v>5232</v>
+      </c>
+      <c r="AC12">
+        <v>5132</v>
+      </c>
+      <c r="AD12">
         <v>4966</v>
-      </c>
-      <c r="E12">
-        <v>5014</v>
-      </c>
-      <c r="F12">
-        <v>4499</v>
-      </c>
-      <c r="G12">
-        <v>5093</v>
-      </c>
-      <c r="H12">
-        <v>5121</v>
-      </c>
-      <c r="I12">
-        <v>5132</v>
-      </c>
-      <c r="J12">
-        <v>5235</v>
-      </c>
-      <c r="K12">
-        <v>4666</v>
-      </c>
-      <c r="L12">
-        <v>4652</v>
-      </c>
-      <c r="M12">
-        <v>4995</v>
-      </c>
-      <c r="N12">
-        <v>4841</v>
-      </c>
-      <c r="O12">
-        <v>4556</v>
-      </c>
-      <c r="P12">
-        <v>5406</v>
-      </c>
-      <c r="Q12">
-        <v>5419</v>
-      </c>
-      <c r="R12">
-        <v>5073</v>
-      </c>
-      <c r="S12">
-        <v>4803</v>
-      </c>
-      <c r="T12">
-        <v>5244</v>
-      </c>
-      <c r="U12">
-        <v>4534</v>
-      </c>
-      <c r="V12">
-        <v>4945</v>
-      </c>
-      <c r="W12">
-        <v>4981</v>
-      </c>
-      <c r="X12">
-        <v>5414</v>
-      </c>
-      <c r="Y12">
-        <v>5288</v>
-      </c>
-      <c r="Z12">
-        <v>4877</v>
-      </c>
-      <c r="AA12">
-        <v>5345</v>
-      </c>
-      <c r="AB12">
-        <v>5299</v>
-      </c>
-      <c r="AC12">
-        <v>4829</v>
-      </c>
-      <c r="AD12">
-        <v>4738</v>
       </c>
       <c r="AE12">
         <v>10</v>
       </c>
       <c r="AF12">
-        <v>280.2214333774951</v>
+        <v>284.3688231614128</v>
       </c>
       <c r="AG12">
-        <v>4993.5</v>
+        <v>5027.4</v>
       </c>
       <c r="AH12">
-        <v>5273.721433377495</v>
+        <v>5311.768823161412</v>
       </c>
       <c r="AI12">
-        <v>4713.278566622505</v>
+        <v>4743.031176838587</v>
       </c>
     </row>
     <row r="13" spans="1:35">
       <c r="A13">
-        <v>5387</v>
+        <v>5125</v>
       </c>
       <c r="B13">
-        <v>4995</v>
+        <v>5088</v>
       </c>
       <c r="C13">
-        <v>4603</v>
+        <v>4559</v>
       </c>
       <c r="D13">
-        <v>5053</v>
+        <v>4592</v>
       </c>
       <c r="E13">
-        <v>5050</v>
+        <v>5151</v>
       </c>
       <c r="F13">
-        <v>4499</v>
+        <v>4852</v>
       </c>
       <c r="G13">
-        <v>5093</v>
+        <v>4737</v>
       </c>
       <c r="H13">
-        <v>5121</v>
+        <v>4890</v>
       </c>
       <c r="I13">
-        <v>5229</v>
+        <v>5245</v>
       </c>
       <c r="J13">
-        <v>5239</v>
+        <v>4980</v>
       </c>
       <c r="K13">
-        <v>4666</v>
+        <v>4972</v>
       </c>
       <c r="L13">
-        <v>4652</v>
+        <v>5021</v>
       </c>
       <c r="M13">
-        <v>5031</v>
+        <v>5339</v>
       </c>
       <c r="N13">
-        <v>4995</v>
+        <v>5399</v>
       </c>
       <c r="O13">
-        <v>4676</v>
+        <v>5605</v>
       </c>
       <c r="P13">
-        <v>5406</v>
+        <v>5015</v>
       </c>
       <c r="Q13">
-        <v>5489</v>
+        <v>5332</v>
       </c>
       <c r="R13">
-        <v>5132</v>
+        <v>5316</v>
       </c>
       <c r="S13">
-        <v>4853</v>
+        <v>4374</v>
       </c>
       <c r="T13">
-        <v>5261</v>
+        <v>5148</v>
       </c>
       <c r="U13">
-        <v>4534</v>
+        <v>5113</v>
       </c>
       <c r="V13">
-        <v>5226</v>
+        <v>5359</v>
       </c>
       <c r="W13">
-        <v>5023</v>
+        <v>4932</v>
       </c>
       <c r="X13">
-        <v>5414</v>
+        <v>4912</v>
       </c>
       <c r="Y13">
-        <v>5288</v>
+        <v>5064</v>
       </c>
       <c r="Z13">
-        <v>4962</v>
+        <v>4984</v>
       </c>
       <c r="AA13">
-        <v>5345</v>
+        <v>4797</v>
       </c>
       <c r="AB13">
-        <v>5299</v>
+        <v>5274</v>
       </c>
       <c r="AC13">
-        <v>4829</v>
+        <v>5215</v>
       </c>
       <c r="AD13">
-        <v>4809</v>
+        <v>4966</v>
       </c>
       <c r="AE13">
         <v>11</v>
       </c>
       <c r="AF13">
-        <v>281.6340843563938</v>
+        <v>268.9003661145736</v>
       </c>
       <c r="AG13">
-        <v>5038.633333333333</v>
+        <v>5045.2</v>
       </c>
       <c r="AH13">
-        <v>5320.267417689727</v>
+        <v>5314.100366114573</v>
       </c>
       <c r="AI13">
-        <v>4756.999248976939</v>
+        <v>4776.299633885426</v>
       </c>
     </row>
     <row r="14" spans="1:35">
       <c r="A14">
-        <v>5448</v>
+        <v>5392</v>
       </c>
       <c r="B14">
-        <v>4995</v>
+        <v>5088</v>
       </c>
       <c r="C14">
-        <v>4603</v>
+        <v>4641</v>
       </c>
       <c r="D14">
+        <v>4592</v>
+      </c>
+      <c r="E14">
+        <v>5151</v>
+      </c>
+      <c r="F14">
+        <v>4852</v>
+      </c>
+      <c r="G14">
+        <v>4765</v>
+      </c>
+      <c r="H14">
         <v>5053</v>
       </c>
-      <c r="E14">
-        <v>5121</v>
-      </c>
-      <c r="F14">
-        <v>4499</v>
-      </c>
-      <c r="G14">
-        <v>5093</v>
-      </c>
-      <c r="H14">
-        <v>5121</v>
-      </c>
       <c r="I14">
-        <v>5351</v>
+        <v>5304</v>
       </c>
       <c r="J14">
-        <v>5239</v>
+        <v>4996</v>
       </c>
       <c r="K14">
-        <v>4666</v>
+        <v>4989</v>
       </c>
       <c r="L14">
-        <v>4715</v>
+        <v>5021</v>
       </c>
       <c r="M14">
-        <v>5031</v>
+        <v>5502</v>
       </c>
       <c r="N14">
-        <v>5054</v>
+        <v>5399</v>
       </c>
       <c r="O14">
-        <v>4689</v>
+        <v>5605</v>
       </c>
       <c r="P14">
-        <v>5406</v>
+        <v>5129</v>
       </c>
       <c r="Q14">
-        <v>5489</v>
+        <v>5332</v>
       </c>
       <c r="R14">
-        <v>5132</v>
+        <v>5316</v>
       </c>
       <c r="S14">
-        <v>4853</v>
+        <v>4619</v>
       </c>
       <c r="T14">
-        <v>5261</v>
+        <v>5153</v>
       </c>
       <c r="U14">
-        <v>4534</v>
+        <v>5127</v>
       </c>
       <c r="V14">
-        <v>5226</v>
+        <v>5398</v>
       </c>
       <c r="W14">
-        <v>5162</v>
+        <v>4932</v>
       </c>
       <c r="X14">
-        <v>5414</v>
+        <v>5292</v>
       </c>
       <c r="Y14">
-        <v>5288</v>
+        <v>5306</v>
       </c>
       <c r="Z14">
-        <v>4962</v>
+        <v>4984</v>
       </c>
       <c r="AA14">
-        <v>5345</v>
+        <v>4884</v>
       </c>
       <c r="AB14">
-        <v>5299</v>
+        <v>5274</v>
       </c>
       <c r="AC14">
-        <v>4852</v>
+        <v>5215</v>
       </c>
       <c r="AD14">
-        <v>4826</v>
+        <v>5032</v>
       </c>
       <c r="AE14">
         <v>12</v>
       </c>
       <c r="AF14">
-        <v>284.4437624961893</v>
+        <v>259.0818913717854</v>
       </c>
       <c r="AG14">
-        <v>5057.566666666667</v>
+        <v>5111.433333333333</v>
       </c>
       <c r="AH14">
-        <v>5342.010429162856</v>
+        <v>5370.515224705119</v>
       </c>
       <c r="AI14">
-        <v>4773.122904170477</v>
+        <v>4852.351441961548</v>
       </c>
     </row>
     <row r="15" spans="1:35">
       <c r="A15">
-        <v>5476</v>
+        <v>5392</v>
       </c>
       <c r="B15">
-        <v>4995</v>
+        <v>5185</v>
       </c>
       <c r="C15">
-        <v>4691</v>
+        <v>4641</v>
       </c>
       <c r="D15">
-        <v>5068</v>
+        <v>4592</v>
       </c>
       <c r="E15">
-        <v>5121</v>
+        <v>5151</v>
       </c>
       <c r="F15">
-        <v>4499</v>
+        <v>4897</v>
       </c>
       <c r="G15">
+        <v>5067</v>
+      </c>
+      <c r="H15">
+        <v>5053</v>
+      </c>
+      <c r="I15">
+        <v>5304</v>
+      </c>
+      <c r="J15">
+        <v>5066</v>
+      </c>
+      <c r="K15">
+        <v>4989</v>
+      </c>
+      <c r="L15">
+        <v>5217</v>
+      </c>
+      <c r="M15">
+        <v>5502</v>
+      </c>
+      <c r="N15">
+        <v>5399</v>
+      </c>
+      <c r="O15">
+        <v>5605</v>
+      </c>
+      <c r="P15">
+        <v>5307</v>
+      </c>
+      <c r="Q15">
+        <v>5441</v>
+      </c>
+      <c r="R15">
+        <v>5316</v>
+      </c>
+      <c r="S15">
+        <v>4767</v>
+      </c>
+      <c r="T15">
+        <v>5153</v>
+      </c>
+      <c r="U15">
+        <v>5163</v>
+      </c>
+      <c r="V15">
+        <v>5446</v>
+      </c>
+      <c r="W15">
+        <v>4932</v>
+      </c>
+      <c r="X15">
+        <v>5292</v>
+      </c>
+      <c r="Y15">
+        <v>5306</v>
+      </c>
+      <c r="Z15">
+        <v>5067</v>
+      </c>
+      <c r="AA15">
+        <v>4953</v>
+      </c>
+      <c r="AB15">
+        <v>5274</v>
+      </c>
+      <c r="AC15">
+        <v>5225</v>
+      </c>
+      <c r="AD15">
         <v>5093</v>
-      </c>
-      <c r="H15">
-        <v>5160</v>
-      </c>
-      <c r="I15">
-        <v>5351</v>
-      </c>
-      <c r="J15">
-        <v>5239</v>
-      </c>
-      <c r="K15">
-        <v>4666</v>
-      </c>
-      <c r="L15">
-        <v>4798</v>
-      </c>
-      <c r="M15">
-        <v>5031</v>
-      </c>
-      <c r="N15">
-        <v>5069</v>
-      </c>
-      <c r="O15">
-        <v>4759</v>
-      </c>
-      <c r="P15">
-        <v>5406</v>
-      </c>
-      <c r="Q15">
-        <v>5506</v>
-      </c>
-      <c r="R15">
-        <v>5132</v>
-      </c>
-      <c r="S15">
-        <v>4853</v>
-      </c>
-      <c r="T15">
-        <v>5313</v>
-      </c>
-      <c r="U15">
-        <v>4534</v>
-      </c>
-      <c r="V15">
-        <v>5226</v>
-      </c>
-      <c r="W15">
-        <v>5162</v>
-      </c>
-      <c r="X15">
-        <v>5414</v>
-      </c>
-      <c r="Y15">
-        <v>5288</v>
-      </c>
-      <c r="Z15">
-        <v>4962</v>
-      </c>
-      <c r="AA15">
-        <v>5365</v>
-      </c>
-      <c r="AB15">
-        <v>5299</v>
-      </c>
-      <c r="AC15">
-        <v>4852</v>
-      </c>
-      <c r="AD15">
-        <v>4956</v>
       </c>
       <c r="AE15">
         <v>13</v>
       </c>
       <c r="AF15">
-        <v>275.6680579264118</v>
+        <v>241.7674977917953</v>
       </c>
       <c r="AG15">
-        <v>5076.133333333333</v>
+        <v>5159.833333333333</v>
       </c>
       <c r="AH15">
-        <v>5351.801391259745</v>
+        <v>5401.600831125128</v>
       </c>
       <c r="AI15">
-        <v>4800.465275406921</v>
+        <v>4918.065835541538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temp solve of RWheel
</commit_message>
<xml_diff>
--- a/log/basline/all.xlsx
+++ b/log/basline/all.xlsx
@@ -591,1179 +591,1179 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2">
-        <v>3909</v>
+        <v>3797</v>
       </c>
       <c r="B2">
-        <v>3962</v>
+        <v>4187</v>
       </c>
       <c r="C2">
-        <v>4335</v>
+        <v>3750</v>
       </c>
       <c r="D2">
-        <v>3892</v>
+        <v>4098</v>
       </c>
       <c r="E2">
-        <v>4133</v>
+        <v>3986</v>
       </c>
       <c r="F2">
-        <v>4138</v>
+        <v>3274</v>
       </c>
       <c r="G2">
-        <v>4526</v>
+        <v>4024</v>
       </c>
       <c r="H2">
-        <v>3685</v>
+        <v>4274</v>
       </c>
       <c r="I2">
-        <v>3879</v>
+        <v>4068</v>
       </c>
       <c r="J2">
-        <v>3676</v>
+        <v>4092</v>
       </c>
       <c r="K2">
-        <v>4009</v>
+        <v>3625</v>
       </c>
       <c r="L2">
-        <v>4101</v>
+        <v>4329</v>
       </c>
       <c r="M2">
-        <v>3997</v>
+        <v>4065</v>
       </c>
       <c r="N2">
-        <v>3769</v>
+        <v>4091</v>
       </c>
       <c r="O2">
-        <v>4233</v>
+        <v>4319</v>
       </c>
       <c r="P2">
-        <v>4130</v>
+        <v>3917</v>
       </c>
       <c r="Q2">
-        <v>3495</v>
+        <v>4302</v>
       </c>
       <c r="R2">
-        <v>3902</v>
+        <v>4058</v>
       </c>
       <c r="S2">
-        <v>3773</v>
+        <v>4206</v>
       </c>
       <c r="T2">
-        <v>4269</v>
+        <v>4357</v>
       </c>
       <c r="U2">
-        <v>4522</v>
+        <v>4370</v>
       </c>
       <c r="V2">
-        <v>3959</v>
+        <v>4171</v>
       </c>
       <c r="W2">
-        <v>4198</v>
+        <v>3974</v>
       </c>
       <c r="X2">
-        <v>3957</v>
+        <v>4004</v>
       </c>
       <c r="Y2">
-        <v>3591</v>
+        <v>4868</v>
       </c>
       <c r="Z2">
-        <v>3990</v>
+        <v>4308</v>
       </c>
       <c r="AA2">
-        <v>3874</v>
+        <v>4278</v>
       </c>
       <c r="AB2">
-        <v>3989</v>
+        <v>4297</v>
       </c>
       <c r="AC2">
-        <v>3978</v>
+        <v>3551</v>
       </c>
       <c r="AD2">
-        <v>3895</v>
+        <v>3960</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>241.9393483414016</v>
+        <v>296.9529549798493</v>
       </c>
       <c r="AG2">
-        <v>3992.2</v>
+        <v>4086.666666666667</v>
       </c>
       <c r="AH2">
-        <v>4234.139348341401</v>
+        <v>4383.619621646516</v>
       </c>
       <c r="AI2">
-        <v>3750.260651658598</v>
+        <v>3789.713711686817</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3">
-        <v>4549</v>
+        <v>3797</v>
       </c>
       <c r="B3">
-        <v>4104</v>
+        <v>4187</v>
       </c>
       <c r="C3">
-        <v>4335</v>
+        <v>3750</v>
       </c>
       <c r="D3">
-        <v>3944</v>
+        <v>4098</v>
       </c>
       <c r="E3">
-        <v>4192</v>
+        <v>3986</v>
       </c>
       <c r="F3">
-        <v>4373</v>
+        <v>3872</v>
       </c>
       <c r="G3">
-        <v>4542</v>
+        <v>4024</v>
       </c>
       <c r="H3">
-        <v>3772</v>
+        <v>4297</v>
       </c>
       <c r="I3">
-        <v>3973</v>
+        <v>4068</v>
       </c>
       <c r="J3">
-        <v>4036</v>
+        <v>4092</v>
       </c>
       <c r="K3">
-        <v>4009</v>
+        <v>3625</v>
       </c>
       <c r="L3">
-        <v>4101</v>
+        <v>4471</v>
       </c>
       <c r="M3">
-        <v>4335</v>
+        <v>4065</v>
       </c>
       <c r="N3">
-        <v>3769</v>
+        <v>4091</v>
       </c>
       <c r="O3">
-        <v>4573</v>
+        <v>4319</v>
       </c>
       <c r="P3">
-        <v>4130</v>
+        <v>3917</v>
       </c>
       <c r="Q3">
-        <v>3874</v>
+        <v>4302</v>
       </c>
       <c r="R3">
-        <v>3992</v>
+        <v>4058</v>
       </c>
       <c r="S3">
-        <v>3827</v>
+        <v>4206</v>
       </c>
       <c r="T3">
-        <v>4269</v>
+        <v>4357</v>
       </c>
       <c r="U3">
-        <v>4522</v>
+        <v>4370</v>
       </c>
       <c r="V3">
-        <v>3959</v>
+        <v>4171</v>
       </c>
       <c r="W3">
-        <v>4519</v>
+        <v>3974</v>
       </c>
       <c r="X3">
-        <v>4013</v>
+        <v>4004</v>
       </c>
       <c r="Y3">
-        <v>3951</v>
+        <v>4868</v>
       </c>
       <c r="Z3">
-        <v>4311</v>
+        <v>4308</v>
       </c>
       <c r="AA3">
-        <v>4009</v>
+        <v>4278</v>
       </c>
       <c r="AB3">
-        <v>4141</v>
+        <v>4297</v>
       </c>
       <c r="AC3">
-        <v>4242</v>
+        <v>3551</v>
       </c>
       <c r="AD3">
-        <v>3949</v>
+        <v>3960</v>
       </c>
       <c r="AE3">
         <v>1</v>
       </c>
       <c r="AF3">
-        <v>241.6876130438848</v>
+        <v>264.0293021878313</v>
       </c>
       <c r="AG3">
-        <v>4143.833333333333</v>
+        <v>4112.1</v>
       </c>
       <c r="AH3">
-        <v>4385.520946377218</v>
+        <v>4376.129302187832</v>
       </c>
       <c r="AI3">
-        <v>3902.145720289448</v>
+        <v>3848.070697812169</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4">
-        <v>4631</v>
+        <v>3797</v>
       </c>
       <c r="B4">
-        <v>4321</v>
+        <v>4187</v>
       </c>
       <c r="C4">
-        <v>4450</v>
+        <v>3750</v>
       </c>
       <c r="D4">
-        <v>3944</v>
+        <v>4098</v>
       </c>
       <c r="E4">
-        <v>4260</v>
+        <v>3986</v>
       </c>
       <c r="F4">
-        <v>4564</v>
+        <v>3872</v>
       </c>
       <c r="G4">
-        <v>4542</v>
+        <v>4024</v>
       </c>
       <c r="H4">
-        <v>3896</v>
+        <v>4297</v>
       </c>
       <c r="I4">
-        <v>4207</v>
+        <v>4068</v>
       </c>
       <c r="J4">
-        <v>4841</v>
+        <v>4092</v>
       </c>
       <c r="K4">
-        <v>4177</v>
+        <v>3938</v>
       </c>
       <c r="L4">
-        <v>4385</v>
+        <v>4471</v>
       </c>
       <c r="M4">
-        <v>4335</v>
+        <v>4065</v>
       </c>
       <c r="N4">
-        <v>3769</v>
+        <v>4091</v>
       </c>
       <c r="O4">
-        <v>4578</v>
+        <v>4319</v>
       </c>
       <c r="P4">
-        <v>4130</v>
+        <v>3917</v>
       </c>
       <c r="Q4">
-        <v>4232</v>
+        <v>4302</v>
       </c>
       <c r="R4">
-        <v>4249</v>
+        <v>4058</v>
       </c>
       <c r="S4">
-        <v>3937</v>
+        <v>4206</v>
       </c>
       <c r="T4">
-        <v>4414</v>
+        <v>4357</v>
       </c>
       <c r="U4">
-        <v>4522</v>
+        <v>4370</v>
       </c>
       <c r="V4">
-        <v>4152</v>
+        <v>4171</v>
       </c>
       <c r="W4">
-        <v>4519</v>
+        <v>3974</v>
       </c>
       <c r="X4">
-        <v>4059</v>
+        <v>4217</v>
       </c>
       <c r="Y4">
-        <v>3951</v>
+        <v>4868</v>
       </c>
       <c r="Z4">
-        <v>4405</v>
+        <v>4308</v>
       </c>
       <c r="AA4">
-        <v>4201</v>
+        <v>4278</v>
       </c>
       <c r="AB4">
-        <v>4416</v>
+        <v>4297</v>
       </c>
       <c r="AC4">
-        <v>4328</v>
+        <v>3551</v>
       </c>
       <c r="AD4">
-        <v>4084</v>
+        <v>3960</v>
       </c>
       <c r="AE4">
         <v>2</v>
       </c>
       <c r="AF4">
-        <v>248.4256844403476</v>
+        <v>249.466531973154</v>
       </c>
       <c r="AG4">
-        <v>4283.3</v>
+        <v>4129.633333333333</v>
       </c>
       <c r="AH4">
-        <v>4531.725684440348</v>
+        <v>4379.099865306487</v>
       </c>
       <c r="AI4">
-        <v>4034.874315559653</v>
+        <v>3880.166801360179</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5">
-        <v>4900</v>
+        <v>3797</v>
       </c>
       <c r="B5">
-        <v>4498</v>
+        <v>4187</v>
       </c>
       <c r="C5">
-        <v>4450</v>
+        <v>4532</v>
       </c>
       <c r="D5">
-        <v>3944</v>
+        <v>4098</v>
       </c>
       <c r="E5">
-        <v>4505</v>
+        <v>3986</v>
       </c>
       <c r="F5">
-        <v>4564</v>
+        <v>3872</v>
       </c>
       <c r="G5">
-        <v>4542</v>
+        <v>4024</v>
       </c>
       <c r="H5">
-        <v>4255</v>
+        <v>4297</v>
       </c>
       <c r="I5">
-        <v>4407</v>
+        <v>4068</v>
       </c>
       <c r="J5">
-        <v>4841</v>
+        <v>4092</v>
       </c>
       <c r="K5">
-        <v>4177</v>
+        <v>3938</v>
       </c>
       <c r="L5">
-        <v>4385</v>
+        <v>4471</v>
       </c>
       <c r="M5">
-        <v>4389</v>
+        <v>4065</v>
       </c>
       <c r="N5">
-        <v>3969</v>
+        <v>4091</v>
       </c>
       <c r="O5">
-        <v>4578</v>
+        <v>4319</v>
       </c>
       <c r="P5">
-        <v>4130</v>
+        <v>3917</v>
       </c>
       <c r="Q5">
-        <v>4484</v>
+        <v>4359</v>
       </c>
       <c r="R5">
-        <v>4352</v>
+        <v>4058</v>
       </c>
       <c r="S5">
-        <v>4243</v>
+        <v>4408</v>
       </c>
       <c r="T5">
-        <v>4468</v>
+        <v>4357</v>
       </c>
       <c r="U5">
-        <v>4739</v>
+        <v>4370</v>
       </c>
       <c r="V5">
-        <v>4202</v>
+        <v>4171</v>
       </c>
       <c r="W5">
-        <v>4748</v>
+        <v>3974</v>
       </c>
       <c r="X5">
-        <v>4386</v>
+        <v>4217</v>
       </c>
       <c r="Y5">
-        <v>4180</v>
+        <v>4868</v>
       </c>
       <c r="Z5">
-        <v>5032</v>
+        <v>4308</v>
       </c>
       <c r="AA5">
-        <v>4513</v>
+        <v>4278</v>
       </c>
       <c r="AB5">
-        <v>4425</v>
+        <v>4297</v>
       </c>
       <c r="AC5">
-        <v>4796</v>
+        <v>3551</v>
       </c>
       <c r="AD5">
-        <v>4725</v>
+        <v>3960</v>
       </c>
       <c r="AE5">
         <v>3</v>
       </c>
       <c r="AF5">
-        <v>263.3047729310578</v>
+        <v>254.6791535724269</v>
       </c>
       <c r="AG5">
-        <v>4460.9</v>
+        <v>4164.333333333333</v>
       </c>
       <c r="AH5">
-        <v>4724.204772931057</v>
+        <v>4419.01248690576</v>
       </c>
       <c r="AI5">
-        <v>4197.595227068942</v>
+        <v>3909.654179760906</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6">
-        <v>4900</v>
+        <v>3797</v>
       </c>
       <c r="B6">
-        <v>4498</v>
+        <v>4187</v>
       </c>
       <c r="C6">
-        <v>4931</v>
+        <v>4532</v>
       </c>
       <c r="D6">
-        <v>3959</v>
+        <v>4098</v>
       </c>
       <c r="E6">
-        <v>4505</v>
+        <v>3986</v>
       </c>
       <c r="F6">
-        <v>4720</v>
+        <v>3872</v>
       </c>
       <c r="G6">
-        <v>4771</v>
+        <v>4024</v>
       </c>
       <c r="H6">
-        <v>4255</v>
+        <v>4297</v>
       </c>
       <c r="I6">
-        <v>4589</v>
+        <v>4068</v>
       </c>
       <c r="J6">
-        <v>4841</v>
+        <v>4092</v>
       </c>
       <c r="K6">
-        <v>4441</v>
+        <v>3938</v>
       </c>
       <c r="L6">
-        <v>4409</v>
+        <v>4471</v>
       </c>
       <c r="M6">
-        <v>4576</v>
+        <v>4065</v>
       </c>
       <c r="N6">
-        <v>3969</v>
+        <v>4091</v>
       </c>
       <c r="O6">
-        <v>4675</v>
+        <v>4319</v>
       </c>
       <c r="P6">
-        <v>4134</v>
+        <v>3917</v>
       </c>
       <c r="Q6">
-        <v>4484</v>
+        <v>4359</v>
       </c>
       <c r="R6">
-        <v>4456</v>
+        <v>4058</v>
       </c>
       <c r="S6">
-        <v>4342</v>
+        <v>4408</v>
       </c>
       <c r="T6">
-        <v>4673</v>
+        <v>4357</v>
       </c>
       <c r="U6">
-        <v>4739</v>
+        <v>4370</v>
       </c>
       <c r="V6">
-        <v>4384</v>
+        <v>4171</v>
       </c>
       <c r="W6">
-        <v>5027</v>
+        <v>3974</v>
       </c>
       <c r="X6">
-        <v>4555</v>
+        <v>4217</v>
       </c>
       <c r="Y6">
-        <v>4303</v>
+        <v>4868</v>
       </c>
       <c r="Z6">
-        <v>5032</v>
+        <v>4467</v>
       </c>
       <c r="AA6">
-        <v>4623</v>
+        <v>4278</v>
       </c>
       <c r="AB6">
-        <v>4435</v>
+        <v>4297</v>
       </c>
       <c r="AC6">
-        <v>4888</v>
+        <v>3551</v>
       </c>
       <c r="AD6">
-        <v>5018</v>
+        <v>3960</v>
       </c>
       <c r="AE6">
         <v>4</v>
       </c>
       <c r="AF6">
-        <v>289.2067549806484</v>
+        <v>259.383019056207</v>
       </c>
       <c r="AG6">
-        <v>4571.066666666667</v>
+        <v>4169.633333333333</v>
       </c>
       <c r="AH6">
-        <v>4860.273421647315</v>
+        <v>4429.01635238954</v>
       </c>
       <c r="AI6">
-        <v>4281.859911686019</v>
+        <v>3910.250314277126</v>
       </c>
     </row>
     <row r="7" spans="1:35">
       <c r="A7">
-        <v>4900</v>
+        <v>3797</v>
       </c>
       <c r="B7">
-        <v>4498</v>
+        <v>4187</v>
       </c>
       <c r="C7">
-        <v>5043</v>
+        <v>4565</v>
       </c>
       <c r="D7">
-        <v>4225</v>
+        <v>4098</v>
       </c>
       <c r="E7">
-        <v>4505</v>
+        <v>3986</v>
       </c>
       <c r="F7">
-        <v>4720</v>
+        <v>3872</v>
       </c>
       <c r="G7">
-        <v>4825</v>
+        <v>4024</v>
       </c>
       <c r="H7">
-        <v>4255</v>
+        <v>4297</v>
       </c>
       <c r="I7">
-        <v>4589</v>
+        <v>4068</v>
       </c>
       <c r="J7">
-        <v>4841</v>
+        <v>4416</v>
       </c>
       <c r="K7">
-        <v>4546</v>
+        <v>3938</v>
       </c>
       <c r="L7">
-        <v>4480</v>
+        <v>4471</v>
       </c>
       <c r="M7">
-        <v>4726</v>
+        <v>4065</v>
       </c>
       <c r="N7">
-        <v>4051</v>
+        <v>4091</v>
       </c>
       <c r="O7">
-        <v>4675</v>
+        <v>4319</v>
       </c>
       <c r="P7">
-        <v>4176</v>
+        <v>3917</v>
       </c>
       <c r="Q7">
-        <v>4484</v>
+        <v>4359</v>
       </c>
       <c r="R7">
-        <v>4586</v>
+        <v>4058</v>
       </c>
       <c r="S7">
-        <v>4342</v>
+        <v>4408</v>
       </c>
       <c r="T7">
-        <v>4673</v>
+        <v>4357</v>
       </c>
       <c r="U7">
-        <v>4785</v>
+        <v>4370</v>
       </c>
       <c r="V7">
-        <v>4386</v>
+        <v>4171</v>
       </c>
       <c r="W7">
-        <v>5027</v>
+        <v>3974</v>
       </c>
       <c r="X7">
-        <v>4983</v>
+        <v>4217</v>
       </c>
       <c r="Y7">
-        <v>4336</v>
+        <v>4868</v>
       </c>
       <c r="Z7">
-        <v>5158</v>
+        <v>4467</v>
       </c>
       <c r="AA7">
-        <v>4857</v>
+        <v>4278</v>
       </c>
       <c r="AB7">
-        <v>4709</v>
+        <v>4297</v>
       </c>
       <c r="AC7">
-        <v>4888</v>
+        <v>3551</v>
       </c>
       <c r="AD7">
-        <v>5170</v>
+        <v>3960</v>
       </c>
       <c r="AE7">
         <v>5</v>
       </c>
       <c r="AF7">
-        <v>293.665477446155</v>
+        <v>264.3491334727922</v>
       </c>
       <c r="AG7">
-        <v>4647.966666666666</v>
+        <v>4181.533333333334</v>
       </c>
       <c r="AH7">
-        <v>4941.632144112821</v>
+        <v>4445.882466806126</v>
       </c>
       <c r="AI7">
-        <v>4354.301189220511</v>
+        <v>3917.184199860541</v>
       </c>
     </row>
     <row r="8" spans="1:35">
       <c r="A8">
-        <v>5372</v>
+        <v>3797</v>
       </c>
       <c r="B8">
-        <v>4517</v>
+        <v>4187</v>
       </c>
       <c r="C8">
-        <v>5199</v>
+        <v>4565</v>
       </c>
       <c r="D8">
-        <v>4225</v>
+        <v>4098</v>
       </c>
       <c r="E8">
-        <v>4505</v>
+        <v>3986</v>
       </c>
       <c r="F8">
-        <v>4742</v>
+        <v>3872</v>
       </c>
       <c r="G8">
-        <v>4825</v>
+        <v>4024</v>
       </c>
       <c r="H8">
-        <v>4255</v>
+        <v>4297</v>
       </c>
       <c r="I8">
-        <v>4589</v>
+        <v>4068</v>
       </c>
       <c r="J8">
-        <v>4841</v>
+        <v>4416</v>
       </c>
       <c r="K8">
-        <v>4546</v>
+        <v>3938</v>
       </c>
       <c r="L8">
-        <v>4635</v>
+        <v>4471</v>
       </c>
       <c r="M8">
-        <v>4726</v>
+        <v>4065</v>
       </c>
       <c r="N8">
-        <v>4051</v>
+        <v>4091</v>
       </c>
       <c r="O8">
-        <v>5111</v>
+        <v>4319</v>
       </c>
       <c r="P8">
-        <v>4176</v>
+        <v>3917</v>
       </c>
       <c r="Q8">
-        <v>4484</v>
+        <v>4359</v>
       </c>
       <c r="R8">
-        <v>4608</v>
+        <v>4058</v>
       </c>
       <c r="S8">
-        <v>4403</v>
+        <v>4408</v>
       </c>
       <c r="T8">
-        <v>4701</v>
+        <v>4357</v>
       </c>
       <c r="U8">
-        <v>4906</v>
+        <v>4370</v>
       </c>
       <c r="V8">
-        <v>4822</v>
+        <v>4171</v>
       </c>
       <c r="W8">
-        <v>5027</v>
+        <v>3974</v>
       </c>
       <c r="X8">
-        <v>4998</v>
+        <v>4217</v>
       </c>
       <c r="Y8">
-        <v>4473</v>
+        <v>4868</v>
       </c>
       <c r="Z8">
-        <v>5158</v>
+        <v>4467</v>
       </c>
       <c r="AA8">
-        <v>4939</v>
+        <v>4278</v>
       </c>
       <c r="AB8">
-        <v>4709</v>
+        <v>4297</v>
       </c>
       <c r="AC8">
-        <v>4888</v>
+        <v>3551</v>
       </c>
       <c r="AD8">
-        <v>5170</v>
+        <v>3960</v>
       </c>
       <c r="AE8">
         <v>6</v>
       </c>
       <c r="AF8">
-        <v>326.8310207002298</v>
+        <v>264.3491334727922</v>
       </c>
       <c r="AG8">
-        <v>4720.033333333334</v>
+        <v>4181.533333333334</v>
       </c>
       <c r="AH8">
-        <v>5046.864354033563</v>
+        <v>4445.882466806126</v>
       </c>
       <c r="AI8">
-        <v>4393.202312633104</v>
+        <v>3917.184199860541</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9">
-        <v>5372</v>
+        <v>3797</v>
       </c>
       <c r="B9">
-        <v>4517</v>
+        <v>4187</v>
       </c>
       <c r="C9">
-        <v>5212</v>
+        <v>4565</v>
       </c>
       <c r="D9">
-        <v>4268</v>
+        <v>4098</v>
       </c>
       <c r="E9">
-        <v>4543</v>
+        <v>4046</v>
       </c>
       <c r="F9">
-        <v>4899</v>
+        <v>3872</v>
       </c>
       <c r="G9">
-        <v>4825</v>
+        <v>4024</v>
       </c>
       <c r="H9">
-        <v>4255</v>
+        <v>4297</v>
       </c>
       <c r="I9">
-        <v>4589</v>
+        <v>4068</v>
       </c>
       <c r="J9">
-        <v>4881</v>
+        <v>4416</v>
       </c>
       <c r="K9">
-        <v>4588</v>
+        <v>3938</v>
       </c>
       <c r="L9">
-        <v>4694</v>
+        <v>4471</v>
       </c>
       <c r="M9">
-        <v>4726</v>
+        <v>4065</v>
       </c>
       <c r="N9">
-        <v>4051</v>
+        <v>4091</v>
       </c>
       <c r="O9">
-        <v>5111</v>
+        <v>4319</v>
       </c>
       <c r="P9">
-        <v>4588</v>
+        <v>3917</v>
       </c>
       <c r="Q9">
-        <v>4705</v>
+        <v>4359</v>
       </c>
       <c r="R9">
-        <v>4608</v>
+        <v>4058</v>
       </c>
       <c r="S9">
-        <v>4403</v>
+        <v>4408</v>
       </c>
       <c r="T9">
-        <v>4829</v>
+        <v>4357</v>
       </c>
       <c r="U9">
-        <v>4906</v>
+        <v>4375</v>
       </c>
       <c r="V9">
-        <v>5126</v>
+        <v>4171</v>
       </c>
       <c r="W9">
-        <v>5027</v>
+        <v>3974</v>
       </c>
       <c r="X9">
-        <v>5214</v>
+        <v>4217</v>
       </c>
       <c r="Y9">
-        <v>4513</v>
+        <v>4868</v>
       </c>
       <c r="Z9">
-        <v>5158</v>
+        <v>4467</v>
       </c>
       <c r="AA9">
-        <v>5085</v>
+        <v>4278</v>
       </c>
       <c r="AB9">
-        <v>4749</v>
+        <v>4297</v>
       </c>
       <c r="AC9">
-        <v>4958</v>
+        <v>3551</v>
       </c>
       <c r="AD9">
-        <v>5245</v>
+        <v>3960</v>
       </c>
       <c r="AE9">
         <v>7</v>
       </c>
       <c r="AF9">
-        <v>327.3123661847674</v>
+        <v>263.1662841312471</v>
       </c>
       <c r="AG9">
-        <v>4788.166666666667</v>
+        <v>4183.7</v>
       </c>
       <c r="AH9">
-        <v>5115.479032851435</v>
+        <v>4446.866284131247</v>
       </c>
       <c r="AI9">
-        <v>4460.854300481899</v>
+        <v>3920.533715868753</v>
       </c>
     </row>
     <row r="10" spans="1:35">
       <c r="A10">
-        <v>5372</v>
+        <v>3797</v>
       </c>
       <c r="B10">
-        <v>4517</v>
+        <v>4187</v>
       </c>
       <c r="C10">
-        <v>5325</v>
+        <v>4565</v>
       </c>
       <c r="D10">
-        <v>4277</v>
+        <v>4098</v>
       </c>
       <c r="E10">
-        <v>4543</v>
+        <v>4046</v>
       </c>
       <c r="F10">
-        <v>4899</v>
+        <v>3872</v>
       </c>
       <c r="G10">
-        <v>4825</v>
+        <v>4024</v>
       </c>
       <c r="H10">
-        <v>4342</v>
+        <v>4297</v>
       </c>
       <c r="I10">
-        <v>4811</v>
+        <v>4068</v>
       </c>
       <c r="J10">
-        <v>4881</v>
+        <v>4416</v>
       </c>
       <c r="K10">
-        <v>4588</v>
+        <v>3938</v>
       </c>
       <c r="L10">
-        <v>4926</v>
+        <v>4471</v>
       </c>
       <c r="M10">
-        <v>4962</v>
+        <v>4065</v>
       </c>
       <c r="N10">
-        <v>4051</v>
+        <v>4091</v>
       </c>
       <c r="O10">
-        <v>5111</v>
+        <v>4319</v>
       </c>
       <c r="P10">
-        <v>4588</v>
+        <v>3917</v>
       </c>
       <c r="Q10">
-        <v>4970</v>
+        <v>4547</v>
       </c>
       <c r="R10">
-        <v>4968</v>
+        <v>4058</v>
       </c>
       <c r="S10">
-        <v>4594</v>
+        <v>4408</v>
       </c>
       <c r="T10">
-        <v>4829</v>
+        <v>4357</v>
       </c>
       <c r="U10">
-        <v>4974</v>
+        <v>4375</v>
       </c>
       <c r="V10">
-        <v>5192</v>
+        <v>4171</v>
       </c>
       <c r="W10">
-        <v>5067</v>
+        <v>3974</v>
       </c>
       <c r="X10">
-        <v>5225</v>
+        <v>4217</v>
       </c>
       <c r="Y10">
-        <v>4831</v>
+        <v>4868</v>
       </c>
       <c r="Z10">
-        <v>5158</v>
+        <v>4467</v>
       </c>
       <c r="AA10">
-        <v>5165</v>
+        <v>4361</v>
       </c>
       <c r="AB10">
-        <v>4977</v>
+        <v>4297</v>
       </c>
       <c r="AC10">
-        <v>4958</v>
+        <v>3551</v>
       </c>
       <c r="AD10">
-        <v>5245</v>
+        <v>3960</v>
       </c>
       <c r="AE10">
         <v>8</v>
       </c>
       <c r="AF10">
-        <v>318.124512961712</v>
+        <v>271.0000551384768</v>
       </c>
       <c r="AG10">
-        <v>4872.366666666667</v>
+        <v>4192.733333333334</v>
       </c>
       <c r="AH10">
-        <v>5190.491179628379</v>
+        <v>4463.73338847181</v>
       </c>
       <c r="AI10">
-        <v>4554.242153704955</v>
+        <v>3921.733278194857</v>
       </c>
     </row>
     <row r="11" spans="1:35">
       <c r="A11">
-        <v>5414</v>
+        <v>3797</v>
       </c>
       <c r="B11">
-        <v>4668</v>
+        <v>4187</v>
       </c>
       <c r="C11">
-        <v>5325</v>
+        <v>4565</v>
       </c>
       <c r="D11">
-        <v>4461</v>
+        <v>4098</v>
       </c>
       <c r="E11">
-        <v>4543</v>
+        <v>4046</v>
       </c>
       <c r="F11">
-        <v>5116</v>
+        <v>3872</v>
       </c>
       <c r="G11">
-        <v>4825</v>
+        <v>4024</v>
       </c>
       <c r="H11">
-        <v>4559</v>
+        <v>4297</v>
       </c>
       <c r="I11">
-        <v>4811</v>
+        <v>4068</v>
       </c>
       <c r="J11">
-        <v>5045</v>
+        <v>4416</v>
       </c>
       <c r="K11">
-        <v>4647</v>
+        <v>3938</v>
       </c>
       <c r="L11">
-        <v>4926</v>
+        <v>4471</v>
       </c>
       <c r="M11">
-        <v>4962</v>
+        <v>4065</v>
       </c>
       <c r="N11">
-        <v>4051</v>
+        <v>4091</v>
       </c>
       <c r="O11">
-        <v>5111</v>
+        <v>4319</v>
       </c>
       <c r="P11">
-        <v>4588</v>
+        <v>3917</v>
       </c>
       <c r="Q11">
-        <v>4970</v>
+        <v>4547</v>
       </c>
       <c r="R11">
-        <v>5114</v>
+        <v>4058</v>
       </c>
       <c r="S11">
-        <v>4594</v>
+        <v>4408</v>
       </c>
       <c r="T11">
-        <v>4867</v>
+        <v>4357</v>
       </c>
       <c r="U11">
-        <v>4974</v>
+        <v>4375</v>
       </c>
       <c r="V11">
-        <v>5192</v>
+        <v>4171</v>
       </c>
       <c r="W11">
-        <v>5127</v>
+        <v>3974</v>
       </c>
       <c r="X11">
-        <v>5381</v>
+        <v>4217</v>
       </c>
       <c r="Y11">
-        <v>4831</v>
+        <v>4868</v>
       </c>
       <c r="Z11">
-        <v>5158</v>
+        <v>4663</v>
       </c>
       <c r="AA11">
-        <v>5173</v>
+        <v>4361</v>
       </c>
       <c r="AB11">
-        <v>4977</v>
+        <v>4297</v>
       </c>
       <c r="AC11">
-        <v>4980</v>
+        <v>3551</v>
       </c>
       <c r="AD11">
-        <v>5245</v>
+        <v>3960</v>
       </c>
       <c r="AE11">
         <v>9</v>
       </c>
       <c r="AF11">
-        <v>306.8379425503074</v>
+        <v>280.0515880226766</v>
       </c>
       <c r="AG11">
-        <v>4921.166666666667</v>
+        <v>4199.266666666666</v>
       </c>
       <c r="AH11">
-        <v>5228.004609216974</v>
+        <v>4479.318254689343</v>
       </c>
       <c r="AI11">
-        <v>4614.32872411636</v>
+        <v>3919.21507864399</v>
       </c>
     </row>
     <row r="12" spans="1:35">
       <c r="A12">
-        <v>5414</v>
+        <v>3797</v>
       </c>
       <c r="B12">
-        <v>4668</v>
+        <v>4187</v>
       </c>
       <c r="C12">
-        <v>5420</v>
+        <v>4565</v>
       </c>
       <c r="D12">
-        <v>4461</v>
+        <v>4098</v>
       </c>
       <c r="E12">
-        <v>4543</v>
+        <v>4046</v>
       </c>
       <c r="F12">
-        <v>5180</v>
+        <v>3872</v>
       </c>
       <c r="G12">
-        <v>4937</v>
+        <v>4024</v>
       </c>
       <c r="H12">
-        <v>4631</v>
+        <v>4297</v>
       </c>
       <c r="I12">
-        <v>4811</v>
+        <v>4068</v>
       </c>
       <c r="J12">
-        <v>5145</v>
+        <v>4416</v>
       </c>
       <c r="K12">
-        <v>4647</v>
+        <v>3938</v>
       </c>
       <c r="L12">
-        <v>5001</v>
+        <v>4471</v>
       </c>
       <c r="M12">
-        <v>4962</v>
+        <v>4065</v>
       </c>
       <c r="N12">
-        <v>4294</v>
+        <v>4091</v>
       </c>
       <c r="O12">
-        <v>5277</v>
+        <v>4319</v>
       </c>
       <c r="P12">
-        <v>4991</v>
+        <v>3917</v>
       </c>
       <c r="Q12">
-        <v>5006</v>
+        <v>4547</v>
       </c>
       <c r="R12">
-        <v>5114</v>
+        <v>4058</v>
       </c>
       <c r="S12">
-        <v>4653</v>
+        <v>4408</v>
       </c>
       <c r="T12">
-        <v>4881</v>
+        <v>4357</v>
       </c>
       <c r="U12">
-        <v>4974</v>
+        <v>4375</v>
       </c>
       <c r="V12">
-        <v>5361</v>
+        <v>4171</v>
       </c>
       <c r="W12">
-        <v>5132</v>
+        <v>3974</v>
       </c>
       <c r="X12">
-        <v>5381</v>
+        <v>4217</v>
       </c>
       <c r="Y12">
-        <v>4831</v>
+        <v>4868</v>
       </c>
       <c r="Z12">
-        <v>5158</v>
+        <v>4663</v>
       </c>
       <c r="AA12">
-        <v>5173</v>
+        <v>4361</v>
       </c>
       <c r="AB12">
-        <v>5046</v>
+        <v>4297</v>
       </c>
       <c r="AC12">
-        <v>4980</v>
+        <v>3551</v>
       </c>
       <c r="AD12">
-        <v>5245</v>
+        <v>3960</v>
       </c>
       <c r="AE12">
         <v>10</v>
       </c>
       <c r="AF12">
-        <v>291.227803159886</v>
+        <v>280.0515880226766</v>
       </c>
       <c r="AG12">
-        <v>4977.233333333334</v>
+        <v>4199.266666666666</v>
       </c>
       <c r="AH12">
-        <v>5268.46113649322</v>
+        <v>4479.318254689343</v>
       </c>
       <c r="AI12">
-        <v>4686.005530173447</v>
+        <v>3919.21507864399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix TSP - out of errors.
</commit_message>
<xml_diff>
--- a/log/basline/all.xlsx
+++ b/log/basline/all.xlsx
@@ -591,1179 +591,1179 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2">
-        <v>3476</v>
+        <v>4398.43020680935</v>
       </c>
       <c r="B2">
-        <v>4063</v>
+        <v>4290.361796875724</v>
       </c>
       <c r="C2">
-        <v>3971</v>
+        <v>4114.784832046243</v>
       </c>
       <c r="D2">
-        <v>4253</v>
+        <v>4254.944274168086</v>
       </c>
       <c r="E2">
-        <v>4401</v>
+        <v>4178.885805142692</v>
       </c>
       <c r="F2">
-        <v>3681</v>
+        <v>4367.620106690559</v>
       </c>
       <c r="G2">
-        <v>3819</v>
+        <v>4032.320600729359</v>
       </c>
       <c r="H2">
-        <v>3765</v>
+        <v>4182.119796911906</v>
       </c>
       <c r="I2">
-        <v>4368</v>
+        <v>4330.699162622797</v>
       </c>
       <c r="J2">
-        <v>4183</v>
+        <v>4329.98560929835</v>
       </c>
       <c r="K2">
-        <v>3780</v>
+        <v>4290.873102831692</v>
       </c>
       <c r="L2">
-        <v>4973</v>
+        <v>4085.191239257138</v>
       </c>
       <c r="M2">
-        <v>4154</v>
+        <v>4113.740063053681</v>
       </c>
       <c r="N2">
-        <v>3213</v>
+        <v>4113.531486898866</v>
       </c>
       <c r="O2">
-        <v>4234</v>
+        <v>3885.644404753759</v>
       </c>
       <c r="P2">
-        <v>3941</v>
+        <v>4368.340131353961</v>
       </c>
       <c r="Q2">
-        <v>4466</v>
+        <v>4245.875114041786</v>
       </c>
       <c r="R2">
-        <v>5037</v>
+        <v>4257.542554456429</v>
       </c>
       <c r="S2">
-        <v>4153</v>
+        <v>4233.283585129627</v>
       </c>
       <c r="T2">
-        <v>3649</v>
+        <v>4149.185064510225</v>
       </c>
       <c r="U2">
-        <v>4178</v>
+        <v>4289.535569812224</v>
       </c>
       <c r="V2">
-        <v>3905</v>
+        <v>4198.545839504756</v>
       </c>
       <c r="W2">
-        <v>3833</v>
+        <v>4194.273506371725</v>
       </c>
       <c r="X2">
-        <v>3885</v>
+        <v>4422.936084921746</v>
       </c>
       <c r="Y2">
-        <v>3891</v>
+        <v>4216.128627752491</v>
       </c>
       <c r="Z2">
-        <v>3473</v>
+        <v>4321.310770455058</v>
       </c>
       <c r="AA2">
-        <v>4033</v>
+        <v>4261.12301975943</v>
       </c>
       <c r="AB2">
-        <v>4100</v>
+        <v>4027.411126602437</v>
       </c>
       <c r="AC2">
-        <v>3787</v>
+        <v>4235.486797775921</v>
       </c>
       <c r="AD2">
-        <v>3816</v>
+        <v>4239.421998365209</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>391.8337511059342</v>
+        <v>119.9499444703725</v>
       </c>
       <c r="AG2">
-        <v>4016.033333333333</v>
+        <v>4220.984409296775</v>
       </c>
       <c r="AH2">
-        <v>4407.867084439267</v>
+        <v>4340.934353767148</v>
       </c>
       <c r="AI2">
-        <v>3624.199582227399</v>
+        <v>4101.034464826403</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3">
-        <v>3716</v>
+        <v>4043.811468923269</v>
       </c>
       <c r="B3">
-        <v>4063</v>
+        <v>4264.722140426434</v>
       </c>
       <c r="C3">
-        <v>3971</v>
+        <v>4114.784832046243</v>
       </c>
       <c r="D3">
-        <v>4253</v>
+        <v>4242.513069197415</v>
       </c>
       <c r="E3">
-        <v>4401</v>
+        <v>4178.885805142692</v>
       </c>
       <c r="F3">
-        <v>3834</v>
+        <v>4293.968268859719</v>
       </c>
       <c r="G3">
-        <v>3819</v>
+        <v>4032.320600729359</v>
       </c>
       <c r="H3">
-        <v>3765</v>
+        <v>4177.315687199358</v>
       </c>
       <c r="I3">
-        <v>4368</v>
+        <v>4109.194807013856</v>
       </c>
       <c r="J3">
-        <v>4183</v>
+        <v>4208.331502926498</v>
       </c>
       <c r="K3">
-        <v>3780</v>
+        <v>4162.81923364564</v>
       </c>
       <c r="L3">
-        <v>4973</v>
+        <v>4085.191239257138</v>
       </c>
       <c r="M3">
-        <v>4154</v>
+        <v>4113.740063053681</v>
       </c>
       <c r="N3">
-        <v>3329</v>
+        <v>4113.531486898866</v>
       </c>
       <c r="O3">
-        <v>4751</v>
+        <v>3885.644404753759</v>
       </c>
       <c r="P3">
-        <v>4218</v>
+        <v>4352.320777739636</v>
       </c>
       <c r="Q3">
-        <v>4466</v>
+        <v>4245.875114041786</v>
       </c>
       <c r="R3">
-        <v>5037</v>
+        <v>4136.71208971015</v>
       </c>
       <c r="S3">
-        <v>4153</v>
+        <v>4161.36506566689</v>
       </c>
       <c r="T3">
-        <v>3659</v>
+        <v>4149.185064510225</v>
       </c>
       <c r="U3">
-        <v>4178</v>
+        <v>4229.735867409958</v>
       </c>
       <c r="V3">
-        <v>3905</v>
+        <v>4198.545839504756</v>
       </c>
       <c r="W3">
-        <v>3833</v>
+        <v>4066.502338727755</v>
       </c>
       <c r="X3">
-        <v>3927</v>
+        <v>4333.814608369932</v>
       </c>
       <c r="Y3">
-        <v>3891</v>
+        <v>4216.128627752491</v>
       </c>
       <c r="Z3">
-        <v>3691</v>
+        <v>4321.310770455058</v>
       </c>
       <c r="AA3">
-        <v>4209</v>
+        <v>4105.214035377197</v>
       </c>
       <c r="AB3">
-        <v>4100</v>
+        <v>4027.411126602437</v>
       </c>
       <c r="AC3">
-        <v>3952</v>
+        <v>4235.486797775921</v>
       </c>
       <c r="AD3">
-        <v>3986</v>
+        <v>4233.858324458168</v>
       </c>
       <c r="AE3">
         <v>1</v>
       </c>
       <c r="AF3">
-        <v>377.1819052594814</v>
+        <v>102.9939020564208</v>
       </c>
       <c r="AG3">
-        <v>4085.5</v>
+        <v>4168.008035272544</v>
       </c>
       <c r="AH3">
-        <v>4462.681905259481</v>
+        <v>4271.001937328964</v>
       </c>
       <c r="AI3">
-        <v>3708.318094740519</v>
+        <v>4065.014133216123</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4">
-        <v>3945</v>
+        <v>4043.811468923269</v>
       </c>
       <c r="B4">
-        <v>4063</v>
+        <v>4182.492051348102</v>
       </c>
       <c r="C4">
-        <v>3971</v>
+        <v>4114.784832046243</v>
       </c>
       <c r="D4">
-        <v>4253</v>
+        <v>4242.513069197415</v>
       </c>
       <c r="E4">
-        <v>4401</v>
+        <v>4178.885805142692</v>
       </c>
       <c r="F4">
-        <v>4290</v>
+        <v>4168.197981837488</v>
       </c>
       <c r="G4">
-        <v>3819</v>
+        <v>4032.320600729359</v>
       </c>
       <c r="H4">
-        <v>4151</v>
+        <v>4148.239638268481</v>
       </c>
       <c r="I4">
-        <v>4368</v>
+        <v>4040.991385841469</v>
       </c>
       <c r="J4">
-        <v>4183</v>
+        <v>4036.612779150249</v>
       </c>
       <c r="K4">
-        <v>3780</v>
+        <v>4162.81923364564</v>
       </c>
       <c r="L4">
-        <v>4973</v>
+        <v>3882.038292339431</v>
       </c>
       <c r="M4">
-        <v>4194</v>
+        <v>4113.740063053681</v>
       </c>
       <c r="N4">
-        <v>3378</v>
+        <v>4113.531486898866</v>
       </c>
       <c r="O4">
-        <v>4751</v>
+        <v>3885.644404753759</v>
       </c>
       <c r="P4">
-        <v>4224</v>
+        <v>4343.541579856456</v>
       </c>
       <c r="Q4">
-        <v>4466</v>
+        <v>4245.875114041786</v>
       </c>
       <c r="R4">
-        <v>5037</v>
+        <v>4136.71208971015</v>
       </c>
       <c r="S4">
-        <v>4369</v>
+        <v>4161.36506566689</v>
       </c>
       <c r="T4">
-        <v>3742</v>
+        <v>3981.336150629966</v>
       </c>
       <c r="U4">
-        <v>4178</v>
+        <v>4191.67548425361</v>
       </c>
       <c r="V4">
-        <v>3973</v>
+        <v>4159.108552782584</v>
       </c>
       <c r="W4">
-        <v>3833</v>
+        <v>4066.502338727755</v>
       </c>
       <c r="X4">
-        <v>4002</v>
+        <v>4152.536524199848</v>
       </c>
       <c r="Y4">
-        <v>4036</v>
+        <v>4134.683637032755</v>
       </c>
       <c r="Z4">
-        <v>3691</v>
+        <v>4302.643575320226</v>
       </c>
       <c r="AA4">
-        <v>4708</v>
+        <v>4105.214035377197</v>
       </c>
       <c r="AB4">
-        <v>4100</v>
+        <v>3950.581415222695</v>
       </c>
       <c r="AC4">
-        <v>4006</v>
+        <v>4235.486797775921</v>
       </c>
       <c r="AD4">
-        <v>3986</v>
+        <v>4233.858324458168</v>
       </c>
       <c r="AE4">
         <v>2</v>
       </c>
       <c r="AF4">
-        <v>368.9681308855758</v>
+        <v>110.0737566868915</v>
       </c>
       <c r="AG4">
-        <v>4162.366666666667</v>
+        <v>4124.924792607739</v>
       </c>
       <c r="AH4">
-        <v>4531.334797552243</v>
+        <v>4234.99854929463</v>
       </c>
       <c r="AI4">
-        <v>3793.398535781091</v>
+        <v>4014.851035920847</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5">
-        <v>3945</v>
+        <v>3979.554928500677</v>
       </c>
       <c r="B5">
-        <v>4602</v>
+        <v>4182.492051348102</v>
       </c>
       <c r="C5">
-        <v>3971</v>
+        <v>4114.784832046243</v>
       </c>
       <c r="D5">
-        <v>4253</v>
+        <v>4242.513069197415</v>
       </c>
       <c r="E5">
-        <v>4401</v>
+        <v>4142.942492509374</v>
       </c>
       <c r="F5">
-        <v>4406</v>
+        <v>4168.197981837488</v>
       </c>
       <c r="G5">
-        <v>4366</v>
+        <v>4032.320600729359</v>
       </c>
       <c r="H5">
-        <v>4151</v>
+        <v>4148.239638268481</v>
       </c>
       <c r="I5">
-        <v>4368</v>
+        <v>4040.991385841469</v>
       </c>
       <c r="J5">
-        <v>4183</v>
+        <v>3938.223653360273</v>
       </c>
       <c r="K5">
-        <v>4052</v>
+        <v>4162.81923364564</v>
       </c>
       <c r="L5">
-        <v>4973</v>
+        <v>3882.038292339431</v>
       </c>
       <c r="M5">
-        <v>4194</v>
+        <v>4108.937863493351</v>
       </c>
       <c r="N5">
-        <v>3842</v>
+        <v>4108.251268283465</v>
       </c>
       <c r="O5">
-        <v>4751</v>
+        <v>3885.644404753759</v>
       </c>
       <c r="P5">
-        <v>4228</v>
+        <v>4288.947294527362</v>
       </c>
       <c r="Q5">
-        <v>4466</v>
+        <v>4245.875114041786</v>
       </c>
       <c r="R5">
-        <v>5037</v>
+        <v>3993.298809462478</v>
       </c>
       <c r="S5">
-        <v>4369</v>
+        <v>4161.36506566689</v>
       </c>
       <c r="T5">
-        <v>3742</v>
+        <v>3981.336150629966</v>
       </c>
       <c r="U5">
-        <v>4482</v>
+        <v>4191.087071822973</v>
       </c>
       <c r="V5">
-        <v>3973</v>
+        <v>4116.962347901228</v>
       </c>
       <c r="W5">
-        <v>4263</v>
+        <v>4066.502338727755</v>
       </c>
       <c r="X5">
-        <v>4002</v>
+        <v>4152.536524199848</v>
       </c>
       <c r="Y5">
-        <v>4036</v>
+        <v>4134.683637032755</v>
       </c>
       <c r="Z5">
-        <v>3691</v>
+        <v>4176.633223453386</v>
       </c>
       <c r="AA5">
-        <v>4708</v>
+        <v>4105.214035377197</v>
       </c>
       <c r="AB5">
-        <v>4100</v>
+        <v>3950.581415222695</v>
       </c>
       <c r="AC5">
-        <v>4136</v>
+        <v>4235.486797775921</v>
       </c>
       <c r="AD5">
-        <v>3986</v>
+        <v>4051.851146753598</v>
       </c>
       <c r="AE5">
         <v>3</v>
       </c>
       <c r="AF5">
-        <v>330.5830116418672</v>
+        <v>106.8718910482536</v>
       </c>
       <c r="AG5">
-        <v>4255.9</v>
+        <v>4099.677088958346</v>
       </c>
       <c r="AH5">
-        <v>4586.483011641867</v>
+        <v>4206.5489800066</v>
       </c>
       <c r="AI5">
-        <v>3925.316988358132</v>
+        <v>3992.805197910092</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6">
-        <v>3945</v>
+        <v>3979.554928500677</v>
       </c>
       <c r="B6">
-        <v>4663</v>
+        <v>4134.834936170226</v>
       </c>
       <c r="C6">
-        <v>4407</v>
+        <v>4114.784832046243</v>
       </c>
       <c r="D6">
-        <v>4253</v>
+        <v>4242.513069197415</v>
       </c>
       <c r="E6">
-        <v>4401</v>
+        <v>4098.780631332637</v>
       </c>
       <c r="F6">
-        <v>4406</v>
+        <v>4168.197981837488</v>
       </c>
       <c r="G6">
-        <v>4366</v>
+        <v>4032.320600729359</v>
       </c>
       <c r="H6">
-        <v>4151</v>
+        <v>4141.828649114111</v>
       </c>
       <c r="I6">
-        <v>4789</v>
+        <v>4040.991385841469</v>
       </c>
       <c r="J6">
-        <v>4460</v>
+        <v>3938.223653360273</v>
       </c>
       <c r="K6">
-        <v>4052</v>
+        <v>4161.364295913424</v>
       </c>
       <c r="L6">
-        <v>4973</v>
+        <v>3751.331342649916</v>
       </c>
       <c r="M6">
-        <v>4194</v>
+        <v>4108.937863493351</v>
       </c>
       <c r="N6">
-        <v>3954</v>
+        <v>4108.251268283465</v>
       </c>
       <c r="O6">
-        <v>4882</v>
+        <v>3885.644404753759</v>
       </c>
       <c r="P6">
-        <v>4295</v>
+        <v>4288.947294527362</v>
       </c>
       <c r="Q6">
-        <v>4466</v>
+        <v>4245.875114041786</v>
       </c>
       <c r="R6">
-        <v>5037</v>
+        <v>3993.298809462478</v>
       </c>
       <c r="S6">
-        <v>4373</v>
+        <v>3979.461954550371</v>
       </c>
       <c r="T6">
-        <v>3743</v>
+        <v>3981.336150629966</v>
       </c>
       <c r="U6">
-        <v>4482</v>
+        <v>4191.087071822973</v>
       </c>
       <c r="V6">
-        <v>4061</v>
+        <v>3951.105791765196</v>
       </c>
       <c r="W6">
-        <v>4263</v>
+        <v>4066.502338727755</v>
       </c>
       <c r="X6">
-        <v>4038</v>
+        <v>4152.536524199848</v>
       </c>
       <c r="Y6">
-        <v>4055</v>
+        <v>4087.816410299291</v>
       </c>
       <c r="Z6">
-        <v>3691</v>
+        <v>4176.633223453386</v>
       </c>
       <c r="AA6">
-        <v>4708</v>
+        <v>4085.082942759929</v>
       </c>
       <c r="AB6">
-        <v>4477</v>
+        <v>3947.81345803351</v>
       </c>
       <c r="AC6">
-        <v>4287</v>
+        <v>4162.080602175031</v>
       </c>
       <c r="AD6">
-        <v>3986</v>
+        <v>3962.329445323629</v>
       </c>
       <c r="AE6">
         <v>4</v>
       </c>
       <c r="AF6">
-        <v>338.2402329298125</v>
+        <v>118.8175682942606</v>
       </c>
       <c r="AG6">
-        <v>4328.6</v>
+        <v>4072.648899166544</v>
       </c>
       <c r="AH6">
-        <v>4666.840232929813</v>
+        <v>4191.466467460805</v>
       </c>
       <c r="AI6">
-        <v>3990.359767070188</v>
+        <v>3953.831330872283</v>
       </c>
     </row>
     <row r="7" spans="1:35">
       <c r="A7">
-        <v>3978</v>
+        <v>3876.504347806812</v>
       </c>
       <c r="B7">
-        <v>4663</v>
+        <v>4112.378057382037</v>
       </c>
       <c r="C7">
-        <v>4407</v>
+        <v>4044.468177775046</v>
       </c>
       <c r="D7">
-        <v>4253</v>
+        <v>4174.175191921611</v>
       </c>
       <c r="E7">
-        <v>4493</v>
+        <v>4083.34828679113</v>
       </c>
       <c r="F7">
-        <v>4406</v>
+        <v>4128.671102361796</v>
       </c>
       <c r="G7">
-        <v>4366</v>
+        <v>4023.433926895607</v>
       </c>
       <c r="H7">
-        <v>4151</v>
+        <v>4139.045239324526</v>
       </c>
       <c r="I7">
-        <v>4969</v>
+        <v>4009.472353879031</v>
       </c>
       <c r="J7">
-        <v>4460</v>
+        <v>3938.223653360273</v>
       </c>
       <c r="K7">
-        <v>4052</v>
+        <v>4161.364295913424</v>
       </c>
       <c r="L7">
-        <v>5103</v>
+        <v>3741.397770715599</v>
       </c>
       <c r="M7">
-        <v>4194</v>
+        <v>4092.714009527802</v>
       </c>
       <c r="N7">
-        <v>3997</v>
+        <v>4108.251268283465</v>
       </c>
       <c r="O7">
-        <v>4893</v>
+        <v>3742.104510259517</v>
       </c>
       <c r="P7">
-        <v>4384</v>
+        <v>4260.964087326761</v>
       </c>
       <c r="Q7">
-        <v>4466</v>
+        <v>4245.875114041786</v>
       </c>
       <c r="R7">
-        <v>5037</v>
+        <v>3993.298809462478</v>
       </c>
       <c r="S7">
-        <v>4617</v>
+        <v>3874.302871801664</v>
       </c>
       <c r="T7">
-        <v>4081</v>
+        <v>3717.908737070632</v>
       </c>
       <c r="U7">
-        <v>4482</v>
+        <v>4176.000855543626</v>
       </c>
       <c r="V7">
-        <v>4061</v>
+        <v>3951.105791765196</v>
       </c>
       <c r="W7">
-        <v>4263</v>
+        <v>4003.881445601857</v>
       </c>
       <c r="X7">
-        <v>4095</v>
+        <v>4152.536524199848</v>
       </c>
       <c r="Y7">
-        <v>4145</v>
+        <v>4086.72813047241</v>
       </c>
       <c r="Z7">
-        <v>3871</v>
+        <v>4176.633223453386</v>
       </c>
       <c r="AA7">
-        <v>4708</v>
+        <v>4085.082942759929</v>
       </c>
       <c r="AB7">
-        <v>4477</v>
+        <v>3947.81345803351</v>
       </c>
       <c r="AC7">
-        <v>4287</v>
+        <v>4162.080602175031</v>
       </c>
       <c r="AD7">
-        <v>3986</v>
+        <v>3962.329445323629</v>
       </c>
       <c r="AE7">
         <v>5</v>
       </c>
       <c r="AF7">
-        <v>329.0275204225359</v>
+        <v>143.6506685124826</v>
       </c>
       <c r="AG7">
-        <v>4378.166666666667</v>
+        <v>4039.069807707647</v>
       </c>
       <c r="AH7">
-        <v>4707.194187089202</v>
+        <v>4182.720476220129</v>
       </c>
       <c r="AI7">
-        <v>4049.139146244131</v>
+        <v>3895.419139195164</v>
       </c>
     </row>
     <row r="8" spans="1:35">
       <c r="A8">
-        <v>4606</v>
+        <v>3876.504347806812</v>
       </c>
       <c r="B8">
-        <v>4663</v>
+        <v>4112.378057382037</v>
       </c>
       <c r="C8">
-        <v>4407</v>
+        <v>4032.430749483882</v>
       </c>
       <c r="D8">
-        <v>4441</v>
+        <v>4148.16025565261</v>
       </c>
       <c r="E8">
-        <v>4493</v>
+        <v>4061.944200590551</v>
       </c>
       <c r="F8">
-        <v>4406</v>
+        <v>4128.671102361796</v>
       </c>
       <c r="G8">
-        <v>4408</v>
+        <v>4023.433926895607</v>
       </c>
       <c r="H8">
-        <v>4399</v>
+        <v>4086.578178276978</v>
       </c>
       <c r="I8">
-        <v>4969</v>
+        <v>3902.286189674337</v>
       </c>
       <c r="J8">
-        <v>4460</v>
+        <v>3938.223653360273</v>
       </c>
       <c r="K8">
-        <v>4052</v>
+        <v>4161.364295913424</v>
       </c>
       <c r="L8">
-        <v>5103</v>
+        <v>3741.397770715599</v>
       </c>
       <c r="M8">
-        <v>4250</v>
+        <v>4092.714009527802</v>
       </c>
       <c r="N8">
-        <v>3997</v>
+        <v>4036.781481655154</v>
       </c>
       <c r="O8">
-        <v>5209</v>
+        <v>3742.104510259517</v>
       </c>
       <c r="P8">
-        <v>4826</v>
+        <v>4193.301722847783</v>
       </c>
       <c r="Q8">
-        <v>4552</v>
+        <v>4083.539854912701</v>
       </c>
       <c r="R8">
-        <v>5037</v>
+        <v>3917.468736119041</v>
       </c>
       <c r="S8">
-        <v>4669</v>
+        <v>3874.302871801664</v>
       </c>
       <c r="T8">
-        <v>4545</v>
+        <v>3717.908737070632</v>
       </c>
       <c r="U8">
-        <v>4482</v>
+        <v>4107.624568105235</v>
       </c>
       <c r="V8">
-        <v>4068</v>
+        <v>3889.409402516725</v>
       </c>
       <c r="W8">
-        <v>4263</v>
+        <v>4003.881445601857</v>
       </c>
       <c r="X8">
-        <v>4398</v>
+        <v>4152.536524199848</v>
       </c>
       <c r="Y8">
-        <v>4402</v>
+        <v>4086.72813047241</v>
       </c>
       <c r="Z8">
-        <v>3871</v>
+        <v>4176.633223453386</v>
       </c>
       <c r="AA8">
-        <v>4708</v>
+        <v>3981.845615351559</v>
       </c>
       <c r="AB8">
-        <v>4480</v>
+        <v>3947.81345803351</v>
       </c>
       <c r="AC8">
-        <v>4662</v>
+        <v>3927.023624666128</v>
       </c>
       <c r="AD8">
-        <v>3986</v>
+        <v>3962.329445323629</v>
       </c>
       <c r="AE8">
         <v>6</v>
       </c>
       <c r="AF8">
-        <v>327.0123833290946</v>
+        <v>131.8070530696905</v>
       </c>
       <c r="AG8">
-        <v>4493.733333333334</v>
+        <v>4003.577336334416</v>
       </c>
       <c r="AH8">
-        <v>4820.745716662428</v>
+        <v>4135.384389404107</v>
       </c>
       <c r="AI8">
-        <v>4166.720950004239</v>
+        <v>3871.770283264726</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9">
-        <v>4613</v>
+        <v>3876.504347806812</v>
       </c>
       <c r="B9">
-        <v>4663</v>
+        <v>4110.918449915516</v>
       </c>
       <c r="C9">
-        <v>4407</v>
+        <v>4032.430749483882</v>
       </c>
       <c r="D9">
-        <v>4441</v>
+        <v>3934.271527403107</v>
       </c>
       <c r="E9">
-        <v>4493</v>
+        <v>4061.944200590551</v>
       </c>
       <c r="F9">
-        <v>4509</v>
+        <v>4105.729879787218</v>
       </c>
       <c r="G9">
-        <v>4449</v>
+        <v>3890.084213346878</v>
       </c>
       <c r="H9">
-        <v>4399</v>
+        <v>4080.148293248155</v>
       </c>
       <c r="I9">
-        <v>4987</v>
+        <v>3902.286189674337</v>
       </c>
       <c r="J9">
-        <v>4460</v>
+        <v>3872.912727445029</v>
       </c>
       <c r="K9">
-        <v>4052</v>
+        <v>4161.364295913424</v>
       </c>
       <c r="L9">
-        <v>5103</v>
+        <v>3741.397770715599</v>
       </c>
       <c r="M9">
-        <v>4250</v>
+        <v>4021.009866910494</v>
       </c>
       <c r="N9">
-        <v>3997</v>
+        <v>4036.781481655154</v>
       </c>
       <c r="O9">
-        <v>5209</v>
+        <v>3742.104510259517</v>
       </c>
       <c r="P9">
-        <v>4826</v>
+        <v>4193.301722847783</v>
       </c>
       <c r="Q9">
-        <v>4552</v>
+        <v>4083.539854912701</v>
       </c>
       <c r="R9">
-        <v>5037</v>
+        <v>3917.468736119041</v>
       </c>
       <c r="S9">
-        <v>4669</v>
+        <v>3874.302871801664</v>
       </c>
       <c r="T9">
-        <v>4545</v>
+        <v>3707.438063422706</v>
       </c>
       <c r="U9">
-        <v>4482</v>
+        <v>4026.648494151807</v>
       </c>
       <c r="V9">
-        <v>4068</v>
+        <v>3889.409402516725</v>
       </c>
       <c r="W9">
-        <v>4263</v>
+        <v>3885.184528486806</v>
       </c>
       <c r="X9">
-        <v>4398</v>
+        <v>4117.643147798251</v>
       </c>
       <c r="Y9">
-        <v>4402</v>
+        <v>4086.72813047241</v>
       </c>
       <c r="Z9">
-        <v>3930</v>
+        <v>4176.633223453386</v>
       </c>
       <c r="AA9">
-        <v>4708</v>
+        <v>3981.845615351559</v>
       </c>
       <c r="AB9">
-        <v>4480</v>
+        <v>3947.81345803351</v>
       </c>
       <c r="AC9">
-        <v>4662</v>
+        <v>3899.788819976822</v>
       </c>
       <c r="AD9">
-        <v>3986</v>
+        <v>3952.860557561129</v>
       </c>
       <c r="AE9">
         <v>7</v>
       </c>
       <c r="AF9">
-        <v>323.5408979459601</v>
+        <v>129.1973340154305</v>
       </c>
       <c r="AG9">
-        <v>4501.333333333333</v>
+        <v>3977.016504368733</v>
       </c>
       <c r="AH9">
-        <v>4824.874231279293</v>
+        <v>4106.213838384164</v>
       </c>
       <c r="AI9">
-        <v>4177.792435387373</v>
+        <v>3847.819170353303</v>
       </c>
     </row>
     <row r="10" spans="1:35">
       <c r="A10">
-        <v>4613</v>
+        <v>3876.504347806812</v>
       </c>
       <c r="B10">
-        <v>4699</v>
+        <v>4059.340755360652</v>
       </c>
       <c r="C10">
-        <v>4515</v>
+        <v>3975.49186220928</v>
       </c>
       <c r="D10">
-        <v>4441</v>
+        <v>3934.271527403107</v>
       </c>
       <c r="E10">
-        <v>4553</v>
+        <v>4061.944200590551</v>
       </c>
       <c r="F10">
-        <v>4509</v>
+        <v>4105.729879787218</v>
       </c>
       <c r="G10">
-        <v>4449</v>
+        <v>3830.308731341631</v>
       </c>
       <c r="H10">
-        <v>4399</v>
+        <v>4080.148293248155</v>
       </c>
       <c r="I10">
-        <v>4987</v>
+        <v>3888.194353691815</v>
       </c>
       <c r="J10">
-        <v>4460</v>
+        <v>3872.912727445029</v>
       </c>
       <c r="K10">
-        <v>4052</v>
+        <v>4161.364295913424</v>
       </c>
       <c r="L10">
-        <v>5121</v>
+        <v>3582.818119354935</v>
       </c>
       <c r="M10">
-        <v>4250</v>
+        <v>4021.009866910494</v>
       </c>
       <c r="N10">
-        <v>3997</v>
+        <v>4036.781481655154</v>
       </c>
       <c r="O10">
-        <v>5209</v>
+        <v>3742.104510259517</v>
       </c>
       <c r="P10">
-        <v>4826</v>
+        <v>4193.301722847783</v>
       </c>
       <c r="Q10">
-        <v>4552</v>
+        <v>4083.539854912701</v>
       </c>
       <c r="R10">
-        <v>5037</v>
+        <v>3917.468736119041</v>
       </c>
       <c r="S10">
-        <v>4694</v>
+        <v>3874.302871801664</v>
       </c>
       <c r="T10">
-        <v>4545</v>
+        <v>3707.438063422706</v>
       </c>
       <c r="U10">
-        <v>4482</v>
+        <v>4008.77341602358</v>
       </c>
       <c r="V10">
-        <v>4102</v>
+        <v>3889.409402516725</v>
       </c>
       <c r="W10">
-        <v>4518</v>
+        <v>3885.184528486806</v>
       </c>
       <c r="X10">
-        <v>4398</v>
+        <v>4117.643147798251</v>
       </c>
       <c r="Y10">
-        <v>4461</v>
+        <v>4060.675531269419</v>
       </c>
       <c r="Z10">
-        <v>4224</v>
+        <v>4176.633223453386</v>
       </c>
       <c r="AA10">
-        <v>4708</v>
+        <v>3981.845615351559</v>
       </c>
       <c r="AB10">
-        <v>4480</v>
+        <v>3904.353809646612</v>
       </c>
       <c r="AC10">
-        <v>4662</v>
+        <v>3899.788819976822</v>
       </c>
       <c r="AD10">
-        <v>3986</v>
+        <v>3952.860557561129</v>
       </c>
       <c r="AE10">
         <v>8</v>
       </c>
       <c r="AF10">
-        <v>305.3867512124453</v>
+        <v>141.1542149771268</v>
       </c>
       <c r="AG10">
-        <v>4530.966666666666</v>
+        <v>3962.738141805532</v>
       </c>
       <c r="AH10">
-        <v>4836.353417879111</v>
+        <v>4103.892356782659</v>
       </c>
       <c r="AI10">
-        <v>4225.579915454221</v>
+        <v>3821.583926828405</v>
       </c>
     </row>
     <row r="11" spans="1:35">
       <c r="A11">
-        <v>4692</v>
+        <v>3860.156550534577</v>
       </c>
       <c r="B11">
-        <v>4699</v>
+        <v>3888.828635297548</v>
       </c>
       <c r="C11">
-        <v>4652</v>
+        <v>3946.290375547124</v>
       </c>
       <c r="D11">
-        <v>4441</v>
+        <v>3934.271527403107</v>
       </c>
       <c r="E11">
-        <v>4553</v>
+        <v>4061.944200590551</v>
       </c>
       <c r="F11">
-        <v>4600</v>
+        <v>4105.729879787218</v>
       </c>
       <c r="G11">
-        <v>4588</v>
+        <v>3830.308731341631</v>
       </c>
       <c r="H11">
-        <v>4399</v>
+        <v>4080.148293248155</v>
       </c>
       <c r="I11">
-        <v>4987</v>
+        <v>3888.194353691815</v>
       </c>
       <c r="J11">
-        <v>4520</v>
+        <v>3872.912727445029</v>
       </c>
       <c r="K11">
-        <v>4052</v>
+        <v>4161.364295913424</v>
       </c>
       <c r="L11">
-        <v>5121</v>
+        <v>3582.818119354935</v>
       </c>
       <c r="M11">
-        <v>4969</v>
+        <v>4021.009866910494</v>
       </c>
       <c r="N11">
-        <v>4059</v>
+        <v>3929.144662485524</v>
       </c>
       <c r="O11">
-        <v>5209</v>
+        <v>3742.104510259517</v>
       </c>
       <c r="P11">
-        <v>4826</v>
+        <v>4036.53995309705</v>
       </c>
       <c r="Q11">
-        <v>4552</v>
+        <v>4023.57917804749</v>
       </c>
       <c r="R11">
-        <v>5037</v>
+        <v>3834.185813160205</v>
       </c>
       <c r="S11">
-        <v>4928</v>
+        <v>3868.628057416159</v>
       </c>
       <c r="T11">
-        <v>4545</v>
+        <v>3707.438063422706</v>
       </c>
       <c r="U11">
-        <v>4482</v>
+        <v>4008.77341602358</v>
       </c>
       <c r="V11">
-        <v>4102</v>
+        <v>3819.228336323561</v>
       </c>
       <c r="W11">
-        <v>4518</v>
+        <v>3885.184528486806</v>
       </c>
       <c r="X11">
-        <v>4398</v>
+        <v>4059.245376128709</v>
       </c>
       <c r="Y11">
-        <v>4480</v>
+        <v>3921.761139931309</v>
       </c>
       <c r="Z11">
-        <v>4224</v>
+        <v>4176.633223453386</v>
       </c>
       <c r="AA11">
-        <v>4708</v>
+        <v>3981.845615351559</v>
       </c>
       <c r="AB11">
-        <v>4480</v>
+        <v>3805.897927000234</v>
       </c>
       <c r="AC11">
-        <v>4676</v>
+        <v>3882.811179538926</v>
       </c>
       <c r="AD11">
-        <v>3986</v>
+        <v>3952.860557561129</v>
       </c>
       <c r="AE11">
         <v>9</v>
       </c>
       <c r="AF11">
-        <v>312.7606425690897</v>
+        <v>132.8430036262417</v>
       </c>
       <c r="AG11">
-        <v>4582.766666666666</v>
+        <v>3928.994636491782</v>
       </c>
       <c r="AH11">
-        <v>4895.527309235757</v>
+        <v>4061.837640118024</v>
       </c>
       <c r="AI11">
-        <v>4270.006024097576</v>
+        <v>3796.151632865541</v>
       </c>
     </row>
     <row r="12" spans="1:35">
       <c r="A12">
-        <v>4893</v>
+        <v>3794.653020043877</v>
       </c>
       <c r="B12">
-        <v>4699</v>
+        <v>3888.828635297548</v>
       </c>
       <c r="C12">
-        <v>4652</v>
+        <v>3906.852602915739</v>
       </c>
       <c r="D12">
-        <v>4441</v>
+        <v>3824.455119146661</v>
       </c>
       <c r="E12">
-        <v>4553</v>
+        <v>4061.944200590551</v>
       </c>
       <c r="F12">
-        <v>4600</v>
+        <v>4105.729879787218</v>
       </c>
       <c r="G12">
-        <v>4588</v>
+        <v>3830.308731341631</v>
       </c>
       <c r="H12">
-        <v>4444</v>
+        <v>4080.148293248155</v>
       </c>
       <c r="I12">
-        <v>4987</v>
+        <v>3888.194353691815</v>
       </c>
       <c r="J12">
-        <v>4520</v>
+        <v>3872.912727445029</v>
       </c>
       <c r="K12">
-        <v>4169</v>
+        <v>4161.364295913424</v>
       </c>
       <c r="L12">
-        <v>5121</v>
+        <v>3582.818119354935</v>
       </c>
       <c r="M12">
-        <v>4969</v>
+        <v>4021.009866910494</v>
       </c>
       <c r="N12">
-        <v>4391</v>
+        <v>3929.144662485524</v>
       </c>
       <c r="O12">
-        <v>5209</v>
+        <v>3730.524520977293</v>
       </c>
       <c r="P12">
-        <v>4826</v>
+        <v>4036.53995309705</v>
       </c>
       <c r="Q12">
-        <v>4552</v>
+        <v>4023.57917804749</v>
       </c>
       <c r="R12">
-        <v>5037</v>
+        <v>3815.950759670592</v>
       </c>
       <c r="S12">
-        <v>4928</v>
+        <v>3857.224278352653</v>
       </c>
       <c r="T12">
-        <v>4545</v>
+        <v>3659.841069047226</v>
       </c>
       <c r="U12">
-        <v>4681</v>
+        <v>4008.77341602358</v>
       </c>
       <c r="V12">
-        <v>4258</v>
+        <v>3767.663951912773</v>
       </c>
       <c r="W12">
-        <v>4531</v>
+        <v>3885.184528486806</v>
       </c>
       <c r="X12">
-        <v>4642</v>
+        <v>4059.245376128709</v>
       </c>
       <c r="Y12">
-        <v>4480</v>
+        <v>3915.688793922054</v>
       </c>
       <c r="Z12">
-        <v>4232</v>
+        <v>3875.242430188273</v>
       </c>
       <c r="AA12">
-        <v>4852</v>
+        <v>3981.845615351559</v>
       </c>
       <c r="AB12">
-        <v>4618</v>
+        <v>3805.897927000234</v>
       </c>
       <c r="AC12">
-        <v>4735</v>
+        <v>3882.811179538926</v>
       </c>
       <c r="AD12">
-        <v>3986</v>
+        <v>3952.860557561129</v>
       </c>
       <c r="AE12">
         <v>10</v>
       </c>
       <c r="AF12">
-        <v>285.5759435600798</v>
+        <v>132.6546871730062</v>
       </c>
       <c r="AG12">
-        <v>4637.966666666666</v>
+        <v>3906.907934782631</v>
       </c>
       <c r="AH12">
-        <v>4923.542610226746</v>
+        <v>4039.562621955637</v>
       </c>
       <c r="AI12">
-        <v>4352.390723106587</v>
+        <v>3774.253247609625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Partially Matched Crossover.
</commit_message>
<xml_diff>
--- a/log/basline/all.xlsx
+++ b/log/basline/all.xlsx
@@ -591,1179 +591,1179 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2">
-        <v>4398.43020680935</v>
+        <v>4182.798651698343</v>
       </c>
       <c r="B2">
-        <v>4290.361796875724</v>
+        <v>4177.597448727024</v>
       </c>
       <c r="C2">
-        <v>4114.784832046243</v>
+        <v>4200.28794797618</v>
       </c>
       <c r="D2">
-        <v>4254.944274168086</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E2">
-        <v>4178.885805142692</v>
+        <v>4363.203762799113</v>
       </c>
       <c r="F2">
-        <v>4367.620106690559</v>
+        <v>4289.313007116892</v>
       </c>
       <c r="G2">
-        <v>4032.320600729359</v>
+        <v>4201.730337248195</v>
       </c>
       <c r="H2">
-        <v>4182.119796911906</v>
+        <v>4220.690002768957</v>
       </c>
       <c r="I2">
-        <v>4330.699162622797</v>
+        <v>4274.010453041199</v>
       </c>
       <c r="J2">
-        <v>4329.98560929835</v>
+        <v>4171.493262381624</v>
       </c>
       <c r="K2">
-        <v>4290.873102831692</v>
+        <v>4301.260950443733</v>
       </c>
       <c r="L2">
-        <v>4085.191239257138</v>
+        <v>4145.857943051519</v>
       </c>
       <c r="M2">
-        <v>4113.740063053681</v>
+        <v>4026.447856934395</v>
       </c>
       <c r="N2">
-        <v>4113.531486898866</v>
+        <v>4166.594010438043</v>
       </c>
       <c r="O2">
-        <v>3885.644404753759</v>
+        <v>4289.854091434014</v>
       </c>
       <c r="P2">
-        <v>4368.340131353961</v>
+        <v>4074.743179163419</v>
       </c>
       <c r="Q2">
-        <v>4245.875114041786</v>
+        <v>4039.820565335298</v>
       </c>
       <c r="R2">
-        <v>4257.542554456429</v>
+        <v>4186.707623829395</v>
       </c>
       <c r="S2">
-        <v>4233.283585129627</v>
+        <v>4233.969700547955</v>
       </c>
       <c r="T2">
-        <v>4149.185064510225</v>
+        <v>4258.591237880026</v>
       </c>
       <c r="U2">
-        <v>4289.535569812224</v>
+        <v>4366.788429377427</v>
       </c>
       <c r="V2">
-        <v>4198.545839504756</v>
+        <v>4335.268898379608</v>
       </c>
       <c r="W2">
-        <v>4194.273506371725</v>
+        <v>4224.603527133314</v>
       </c>
       <c r="X2">
-        <v>4422.936084921746</v>
+        <v>4113.490509519408</v>
       </c>
       <c r="Y2">
-        <v>4216.128627752491</v>
+        <v>4339.821745983342</v>
       </c>
       <c r="Z2">
-        <v>4321.310770455058</v>
+        <v>4122.760395925205</v>
       </c>
       <c r="AA2">
-        <v>4261.12301975943</v>
+        <v>4220.187870242893</v>
       </c>
       <c r="AB2">
-        <v>4027.411126602437</v>
+        <v>4320.14475225888</v>
       </c>
       <c r="AC2">
-        <v>4235.486797775921</v>
+        <v>4403.692141776349</v>
       </c>
       <c r="AD2">
-        <v>4239.421998365209</v>
+        <v>4080.767182948651</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>119.9499444703725</v>
+        <v>116.2910617676466</v>
       </c>
       <c r="AG2">
-        <v>4220.984409296775</v>
+        <v>4207.068868700875</v>
       </c>
       <c r="AH2">
-        <v>4340.934353767148</v>
+        <v>4323.359930468522</v>
       </c>
       <c r="AI2">
-        <v>4101.034464826403</v>
+        <v>4090.777806933228</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3">
-        <v>4043.811468923269</v>
+        <v>4182.798651698343</v>
       </c>
       <c r="B3">
-        <v>4264.722140426434</v>
+        <v>4177.597448727024</v>
       </c>
       <c r="C3">
-        <v>4114.784832046243</v>
+        <v>4200.28794797618</v>
       </c>
       <c r="D3">
-        <v>4242.513069197415</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E3">
-        <v>4178.885805142692</v>
+        <v>4363.203762799113</v>
       </c>
       <c r="F3">
-        <v>4293.968268859719</v>
+        <v>4280.169215615671</v>
       </c>
       <c r="G3">
-        <v>4032.320600729359</v>
+        <v>4201.730337248195</v>
       </c>
       <c r="H3">
-        <v>4177.315687199358</v>
+        <v>4220.690002768957</v>
       </c>
       <c r="I3">
-        <v>4109.194807013856</v>
+        <v>4109.967060358828</v>
       </c>
       <c r="J3">
-        <v>4208.331502926498</v>
+        <v>4066.41872927242</v>
       </c>
       <c r="K3">
-        <v>4162.81923364564</v>
+        <v>4301.260950443733</v>
       </c>
       <c r="L3">
-        <v>4085.191239257138</v>
+        <v>4071.457736692125</v>
       </c>
       <c r="M3">
-        <v>4113.740063053681</v>
+        <v>4003.936478312752</v>
       </c>
       <c r="N3">
-        <v>4113.531486898866</v>
+        <v>4166.594010438043</v>
       </c>
       <c r="O3">
-        <v>3885.644404753759</v>
+        <v>4272.842298340157</v>
       </c>
       <c r="P3">
-        <v>4352.320777739636</v>
+        <v>4074.743179163419</v>
       </c>
       <c r="Q3">
-        <v>4245.875114041786</v>
+        <v>4039.820565335298</v>
       </c>
       <c r="R3">
-        <v>4136.71208971015</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S3">
-        <v>4161.36506566689</v>
+        <v>4233.969700547955</v>
       </c>
       <c r="T3">
-        <v>4149.185064510225</v>
+        <v>4234.383934797102</v>
       </c>
       <c r="U3">
-        <v>4229.735867409958</v>
+        <v>4366.788429377427</v>
       </c>
       <c r="V3">
-        <v>4198.545839504756</v>
+        <v>4276.118057490181</v>
       </c>
       <c r="W3">
-        <v>4066.502338727755</v>
+        <v>4110.151735092823</v>
       </c>
       <c r="X3">
-        <v>4333.814608369932</v>
+        <v>4113.490509519408</v>
       </c>
       <c r="Y3">
-        <v>4216.128627752491</v>
+        <v>4210.617293134998</v>
       </c>
       <c r="Z3">
-        <v>4321.310770455058</v>
+        <v>4122.760395925205</v>
       </c>
       <c r="AA3">
-        <v>4105.214035377197</v>
+        <v>4220.187870242893</v>
       </c>
       <c r="AB3">
-        <v>4027.411126602437</v>
+        <v>4320.14475225888</v>
       </c>
       <c r="AC3">
-        <v>4235.486797775921</v>
+        <v>4403.692141776349</v>
       </c>
       <c r="AD3">
-        <v>4233.858324458168</v>
+        <v>4080.767182948651</v>
       </c>
       <c r="AE3">
         <v>1</v>
       </c>
       <c r="AF3">
-        <v>102.9939020564208</v>
+        <v>117.0800051589779</v>
       </c>
       <c r="AG3">
-        <v>4168.008035272544</v>
+        <v>4181.494560990232</v>
       </c>
       <c r="AH3">
-        <v>4271.001937328964</v>
+        <v>4298.57456614921</v>
       </c>
       <c r="AI3">
-        <v>4065.014133216123</v>
+        <v>4064.414555831254</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4">
-        <v>4043.811468923269</v>
+        <v>4121.041849907148</v>
       </c>
       <c r="B4">
-        <v>4182.492051348102</v>
+        <v>4022.994289493579</v>
       </c>
       <c r="C4">
-        <v>4114.784832046243</v>
+        <v>4200.28794797618</v>
       </c>
       <c r="D4">
-        <v>4242.513069197415</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E4">
-        <v>4178.885805142692</v>
+        <v>4363.203762799113</v>
       </c>
       <c r="F4">
-        <v>4168.197981837488</v>
+        <v>4280.169215615671</v>
       </c>
       <c r="G4">
-        <v>4032.320600729359</v>
+        <v>4153.802161834338</v>
       </c>
       <c r="H4">
-        <v>4148.239638268481</v>
+        <v>4167.734760263412</v>
       </c>
       <c r="I4">
-        <v>4040.991385841469</v>
+        <v>4105.498121553924</v>
       </c>
       <c r="J4">
-        <v>4036.612779150249</v>
+        <v>4039.985827795884</v>
       </c>
       <c r="K4">
-        <v>4162.81923364564</v>
+        <v>4301.260950443733</v>
       </c>
       <c r="L4">
-        <v>3882.038292339431</v>
+        <v>4024.627038190148</v>
       </c>
       <c r="M4">
-        <v>4113.740063053681</v>
+        <v>4002.722642646088</v>
       </c>
       <c r="N4">
-        <v>4113.531486898866</v>
+        <v>4163.662193025788</v>
       </c>
       <c r="O4">
-        <v>3885.644404753759</v>
+        <v>4211.445205727659</v>
       </c>
       <c r="P4">
-        <v>4343.541579856456</v>
+        <v>4074.743179163419</v>
       </c>
       <c r="Q4">
-        <v>4245.875114041786</v>
+        <v>4037.565481702095</v>
       </c>
       <c r="R4">
-        <v>4136.71208971015</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S4">
-        <v>4161.36506566689</v>
+        <v>4233.969700547955</v>
       </c>
       <c r="T4">
-        <v>3981.336150629966</v>
+        <v>4234.383934797102</v>
       </c>
       <c r="U4">
-        <v>4191.67548425361</v>
+        <v>4366.788429377427</v>
       </c>
       <c r="V4">
-        <v>4159.108552782584</v>
+        <v>4276.118057490181</v>
       </c>
       <c r="W4">
-        <v>4066.502338727755</v>
+        <v>4103.94636274034</v>
       </c>
       <c r="X4">
-        <v>4152.536524199848</v>
+        <v>3998.138070531252</v>
       </c>
       <c r="Y4">
-        <v>4134.683637032755</v>
+        <v>4141.63110474518</v>
       </c>
       <c r="Z4">
-        <v>4302.643575320226</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA4">
-        <v>4105.214035377197</v>
+        <v>4155.292172714396</v>
       </c>
       <c r="AB4">
-        <v>3950.581415222695</v>
+        <v>4262.024763711572</v>
       </c>
       <c r="AC4">
-        <v>4235.486797775921</v>
+        <v>4374.970396024968</v>
       </c>
       <c r="AD4">
-        <v>4233.858324458168</v>
+        <v>4080.767182948651</v>
       </c>
       <c r="AE4">
         <v>2</v>
       </c>
       <c r="AF4">
-        <v>110.0737566868915</v>
+        <v>132.0802404804336</v>
       </c>
       <c r="AG4">
-        <v>4124.924792607739</v>
+        <v>4145.907889395475</v>
       </c>
       <c r="AH4">
-        <v>4234.99854929463</v>
+        <v>4277.988129875908</v>
       </c>
       <c r="AI4">
-        <v>4014.851035920847</v>
+        <v>4013.827648915041</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5">
-        <v>3979.554928500677</v>
+        <v>4121.041849907148</v>
       </c>
       <c r="B5">
-        <v>4182.492051348102</v>
+        <v>4021.268557446408</v>
       </c>
       <c r="C5">
-        <v>4114.784832046243</v>
+        <v>4200.28794797618</v>
       </c>
       <c r="D5">
-        <v>4242.513069197415</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E5">
-        <v>4142.942492509374</v>
+        <v>4363.203762799113</v>
       </c>
       <c r="F5">
-        <v>4168.197981837488</v>
+        <v>4280.169215615671</v>
       </c>
       <c r="G5">
-        <v>4032.320600729359</v>
+        <v>4098.736683771019</v>
       </c>
       <c r="H5">
-        <v>4148.239638268481</v>
+        <v>4167.734760263412</v>
       </c>
       <c r="I5">
-        <v>4040.991385841469</v>
+        <v>4011.262884979989</v>
       </c>
       <c r="J5">
-        <v>3938.223653360273</v>
+        <v>4039.985827795884</v>
       </c>
       <c r="K5">
-        <v>4162.81923364564</v>
+        <v>4256.403088904978</v>
       </c>
       <c r="L5">
-        <v>3882.038292339431</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M5">
-        <v>4108.937863493351</v>
+        <v>4002.722642646088</v>
       </c>
       <c r="N5">
-        <v>4108.251268283465</v>
+        <v>4163.662193025788</v>
       </c>
       <c r="O5">
-        <v>3885.644404753759</v>
+        <v>4211.445205727659</v>
       </c>
       <c r="P5">
-        <v>4288.947294527362</v>
+        <v>4074.743179163419</v>
       </c>
       <c r="Q5">
-        <v>4245.875114041786</v>
+        <v>4028.797655952813</v>
       </c>
       <c r="R5">
-        <v>3993.298809462478</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S5">
-        <v>4161.36506566689</v>
+        <v>4233.969700547955</v>
       </c>
       <c r="T5">
-        <v>3981.336150629966</v>
+        <v>4202.57169580428</v>
       </c>
       <c r="U5">
-        <v>4191.087071822973</v>
+        <v>4218.47708522146</v>
       </c>
       <c r="V5">
-        <v>4116.962347901228</v>
+        <v>4114.02442874095</v>
       </c>
       <c r="W5">
-        <v>4066.502338727755</v>
+        <v>4103.94636274034</v>
       </c>
       <c r="X5">
-        <v>4152.536524199848</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y5">
-        <v>4134.683637032755</v>
+        <v>4141.63110474518</v>
       </c>
       <c r="Z5">
-        <v>4176.633223453386</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA5">
-        <v>4105.214035377197</v>
+        <v>4155.292172714396</v>
       </c>
       <c r="AB5">
-        <v>3950.581415222695</v>
+        <v>4113.425971195736</v>
       </c>
       <c r="AC5">
-        <v>4235.486797775921</v>
+        <v>4320.451493906685</v>
       </c>
       <c r="AD5">
-        <v>4051.851146753598</v>
+        <v>4080.767182948651</v>
       </c>
       <c r="AE5">
         <v>3</v>
       </c>
       <c r="AF5">
-        <v>106.8718910482536</v>
+        <v>120.4157122588329</v>
       </c>
       <c r="AG5">
-        <v>4099.677088958346</v>
+        <v>4118.251483102275</v>
       </c>
       <c r="AH5">
-        <v>4206.5489800066</v>
+        <v>4238.667195361108</v>
       </c>
       <c r="AI5">
-        <v>3992.805197910092</v>
+        <v>3997.835770843442</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6">
-        <v>3979.554928500677</v>
+        <v>4073.150973979763</v>
       </c>
       <c r="B6">
-        <v>4134.834936170226</v>
+        <v>4021.268557446408</v>
       </c>
       <c r="C6">
-        <v>4114.784832046243</v>
+        <v>4181.072717457391</v>
       </c>
       <c r="D6">
-        <v>4242.513069197415</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E6">
-        <v>4098.780631332637</v>
+        <v>4277.040679972994</v>
       </c>
       <c r="F6">
-        <v>4168.197981837488</v>
+        <v>4090.507436366653</v>
       </c>
       <c r="G6">
-        <v>4032.320600729359</v>
+        <v>4098.736683771019</v>
       </c>
       <c r="H6">
-        <v>4141.828649114111</v>
+        <v>4165.596755217855</v>
       </c>
       <c r="I6">
-        <v>4040.991385841469</v>
+        <v>4011.262884979989</v>
       </c>
       <c r="J6">
-        <v>3938.223653360273</v>
+        <v>4039.985827795884</v>
       </c>
       <c r="K6">
-        <v>4161.364295913424</v>
+        <v>4256.403088904978</v>
       </c>
       <c r="L6">
-        <v>3751.331342649916</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M6">
-        <v>4108.937863493351</v>
+        <v>4002.722642646088</v>
       </c>
       <c r="N6">
-        <v>4108.251268283465</v>
+        <v>4143.202917589537</v>
       </c>
       <c r="O6">
-        <v>3885.644404753759</v>
+        <v>4211.445205727659</v>
       </c>
       <c r="P6">
-        <v>4288.947294527362</v>
+        <v>4056.227724279861</v>
       </c>
       <c r="Q6">
-        <v>4245.875114041786</v>
+        <v>4028.797655952813</v>
       </c>
       <c r="R6">
-        <v>3993.298809462478</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S6">
-        <v>3979.461954550371</v>
+        <v>4233.969700547955</v>
       </c>
       <c r="T6">
-        <v>3981.336150629966</v>
+        <v>3997.946913772582</v>
       </c>
       <c r="U6">
-        <v>4191.087071822973</v>
+        <v>4218.47708522146</v>
       </c>
       <c r="V6">
-        <v>3951.105791765196</v>
+        <v>4088.449422597257</v>
       </c>
       <c r="W6">
-        <v>4066.502338727755</v>
+        <v>4103.94636274034</v>
       </c>
       <c r="X6">
-        <v>4152.536524199848</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y6">
-        <v>4087.816410299291</v>
+        <v>4141.63110474518</v>
       </c>
       <c r="Z6">
-        <v>4176.633223453386</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA6">
-        <v>4085.082942759929</v>
+        <v>4096.138654316387</v>
       </c>
       <c r="AB6">
-        <v>3947.81345803351</v>
+        <v>4113.425971195736</v>
       </c>
       <c r="AC6">
-        <v>4162.080602175031</v>
+        <v>4003.267882252596</v>
       </c>
       <c r="AD6">
-        <v>3962.329445323629</v>
+        <v>4080.767182948651</v>
       </c>
       <c r="AE6">
         <v>4</v>
       </c>
       <c r="AF6">
-        <v>118.8175682942606</v>
+        <v>102.8544221348295</v>
       </c>
       <c r="AG6">
-        <v>4072.648899166544</v>
+        <v>4085.232129031803</v>
       </c>
       <c r="AH6">
-        <v>4191.466467460805</v>
+        <v>4188.086551166632</v>
       </c>
       <c r="AI6">
-        <v>3953.831330872283</v>
+        <v>3982.377706896973</v>
       </c>
     </row>
     <row r="7" spans="1:35">
       <c r="A7">
-        <v>3876.504347806812</v>
+        <v>4073.150973979763</v>
       </c>
       <c r="B7">
-        <v>4112.378057382037</v>
+        <v>4008.519560781017</v>
       </c>
       <c r="C7">
-        <v>4044.468177775046</v>
+        <v>4181.072717457391</v>
       </c>
       <c r="D7">
-        <v>4174.175191921611</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E7">
-        <v>4083.34828679113</v>
+        <v>4277.040679972994</v>
       </c>
       <c r="F7">
-        <v>4128.671102361796</v>
+        <v>4090.507436366653</v>
       </c>
       <c r="G7">
-        <v>4023.433926895607</v>
+        <v>4098.736683771019</v>
       </c>
       <c r="H7">
-        <v>4139.045239324526</v>
+        <v>4165.596755217855</v>
       </c>
       <c r="I7">
-        <v>4009.472353879031</v>
+        <v>4011.262884979989</v>
       </c>
       <c r="J7">
-        <v>3938.223653360273</v>
+        <v>4039.985827795884</v>
       </c>
       <c r="K7">
-        <v>4161.364295913424</v>
+        <v>4060.687041401625</v>
       </c>
       <c r="L7">
-        <v>3741.397770715599</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M7">
-        <v>4092.714009527802</v>
+        <v>3996.998694298975</v>
       </c>
       <c r="N7">
-        <v>4108.251268283465</v>
+        <v>3962.055252700118</v>
       </c>
       <c r="O7">
-        <v>3742.104510259517</v>
+        <v>4211.445205727659</v>
       </c>
       <c r="P7">
-        <v>4260.964087326761</v>
+        <v>4056.227724279861</v>
       </c>
       <c r="Q7">
-        <v>4245.875114041786</v>
+        <v>4028.797655952813</v>
       </c>
       <c r="R7">
-        <v>3993.298809462478</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S7">
-        <v>3874.302871801664</v>
+        <v>4207.059823072322</v>
       </c>
       <c r="T7">
-        <v>3717.908737070632</v>
+        <v>3997.946913772582</v>
       </c>
       <c r="U7">
-        <v>4176.000855543626</v>
+        <v>4218.47708522146</v>
       </c>
       <c r="V7">
-        <v>3951.105791765196</v>
+        <v>4088.449422597257</v>
       </c>
       <c r="W7">
-        <v>4003.881445601857</v>
+        <v>4103.94636274034</v>
       </c>
       <c r="X7">
-        <v>4152.536524199848</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y7">
-        <v>4086.72813047241</v>
+        <v>4141.63110474518</v>
       </c>
       <c r="Z7">
-        <v>4176.633223453386</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA7">
-        <v>4085.082942759929</v>
+        <v>4096.138654316387</v>
       </c>
       <c r="AB7">
-        <v>3947.81345803351</v>
+        <v>4113.425971195736</v>
       </c>
       <c r="AC7">
-        <v>4162.080602175031</v>
+        <v>4003.267882252596</v>
       </c>
       <c r="AD7">
-        <v>3962.329445323629</v>
+        <v>4062.713382010994</v>
       </c>
       <c r="AE7">
         <v>5</v>
       </c>
       <c r="AF7">
-        <v>143.6506685124826</v>
+        <v>98.15922391957838</v>
       </c>
       <c r="AG7">
-        <v>4039.069807707647</v>
+        <v>4070.555451171184</v>
       </c>
       <c r="AH7">
-        <v>4182.720476220129</v>
+        <v>4168.714675090762</v>
       </c>
       <c r="AI7">
-        <v>3895.419139195164</v>
+        <v>3972.396227251606</v>
       </c>
     </row>
     <row r="8" spans="1:35">
       <c r="A8">
-        <v>3876.504347806812</v>
+        <v>4073.150973979763</v>
       </c>
       <c r="B8">
-        <v>4112.378057382037</v>
+        <v>3961.743297273461</v>
       </c>
       <c r="C8">
-        <v>4032.430749483882</v>
+        <v>4181.072717457391</v>
       </c>
       <c r="D8">
-        <v>4148.16025565261</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E8">
-        <v>4061.944200590551</v>
+        <v>4271.792090327821</v>
       </c>
       <c r="F8">
-        <v>4128.671102361796</v>
+        <v>4090.507436366653</v>
       </c>
       <c r="G8">
-        <v>4023.433926895607</v>
+        <v>4098.736683771019</v>
       </c>
       <c r="H8">
-        <v>4086.578178276978</v>
+        <v>4165.596755217855</v>
       </c>
       <c r="I8">
-        <v>3902.286189674337</v>
+        <v>4011.262884979989</v>
       </c>
       <c r="J8">
-        <v>3938.223653360273</v>
+        <v>4039.985827795884</v>
       </c>
       <c r="K8">
-        <v>4161.364295913424</v>
+        <v>4060.687041401625</v>
       </c>
       <c r="L8">
-        <v>3741.397770715599</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M8">
-        <v>4092.714009527802</v>
+        <v>3951.525545262272</v>
       </c>
       <c r="N8">
-        <v>4036.781481655154</v>
+        <v>3962.055252700118</v>
       </c>
       <c r="O8">
-        <v>3742.104510259517</v>
+        <v>4090.793752666073</v>
       </c>
       <c r="P8">
-        <v>4193.301722847783</v>
+        <v>3987.020649790948</v>
       </c>
       <c r="Q8">
-        <v>4083.539854912701</v>
+        <v>4028.797655952813</v>
       </c>
       <c r="R8">
-        <v>3917.468736119041</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S8">
-        <v>3874.302871801664</v>
+        <v>4207.059823072322</v>
       </c>
       <c r="T8">
-        <v>3717.908737070632</v>
+        <v>3997.946913772582</v>
       </c>
       <c r="U8">
-        <v>4107.624568105235</v>
+        <v>4021.217076499784</v>
       </c>
       <c r="V8">
-        <v>3889.409402516725</v>
+        <v>4088.449422597257</v>
       </c>
       <c r="W8">
-        <v>4003.881445601857</v>
+        <v>4103.94636274034</v>
       </c>
       <c r="X8">
-        <v>4152.536524199848</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y8">
-        <v>4086.72813047241</v>
+        <v>4141.63110474518</v>
       </c>
       <c r="Z8">
-        <v>4176.633223453386</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA8">
-        <v>3981.845615351559</v>
+        <v>4054.805089244566</v>
       </c>
       <c r="AB8">
-        <v>3947.81345803351</v>
+        <v>3995.127283963309</v>
       </c>
       <c r="AC8">
-        <v>3927.023624666128</v>
+        <v>4003.267882252596</v>
       </c>
       <c r="AD8">
-        <v>3962.329445323629</v>
+        <v>4062.713382010994</v>
       </c>
       <c r="AE8">
         <v>6</v>
       </c>
       <c r="AF8">
-        <v>131.8070530696905</v>
+        <v>93.13074766732913</v>
       </c>
       <c r="AG8">
-        <v>4003.577336334416</v>
+        <v>4049.080491478989</v>
       </c>
       <c r="AH8">
-        <v>4135.384389404107</v>
+        <v>4142.211239146318</v>
       </c>
       <c r="AI8">
-        <v>3871.770283264726</v>
+        <v>3955.94974381166</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9">
-        <v>3876.504347806812</v>
+        <v>4073.150973979763</v>
       </c>
       <c r="B9">
-        <v>4110.918449915516</v>
+        <v>3961.743297273461</v>
       </c>
       <c r="C9">
-        <v>4032.430749483882</v>
+        <v>4181.072717457391</v>
       </c>
       <c r="D9">
-        <v>3934.271527403107</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E9">
-        <v>4061.944200590551</v>
+        <v>4211.169281233559</v>
       </c>
       <c r="F9">
-        <v>4105.729879787218</v>
+        <v>4076.13586166109</v>
       </c>
       <c r="G9">
-        <v>3890.084213346878</v>
+        <v>3963.054608463689</v>
       </c>
       <c r="H9">
-        <v>4080.148293248155</v>
+        <v>4165.596755217855</v>
       </c>
       <c r="I9">
-        <v>3902.286189674337</v>
+        <v>4011.262884979989</v>
       </c>
       <c r="J9">
-        <v>3872.912727445029</v>
+        <v>3957.067505419134</v>
       </c>
       <c r="K9">
-        <v>4161.364295913424</v>
+        <v>4060.687041401625</v>
       </c>
       <c r="L9">
-        <v>3741.397770715599</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M9">
-        <v>4021.009866910494</v>
+        <v>3857.687076954601</v>
       </c>
       <c r="N9">
-        <v>4036.781481655154</v>
+        <v>3957.918244635269</v>
       </c>
       <c r="O9">
-        <v>3742.104510259517</v>
+        <v>4090.793752666073</v>
       </c>
       <c r="P9">
-        <v>4193.301722847783</v>
+        <v>3987.020649790948</v>
       </c>
       <c r="Q9">
-        <v>4083.539854912701</v>
+        <v>4028.797655952813</v>
       </c>
       <c r="R9">
-        <v>3917.468736119041</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S9">
-        <v>3874.302871801664</v>
+        <v>4207.059823072322</v>
       </c>
       <c r="T9">
-        <v>3707.438063422706</v>
+        <v>3997.946913772582</v>
       </c>
       <c r="U9">
-        <v>4026.648494151807</v>
+        <v>4021.217076499784</v>
       </c>
       <c r="V9">
-        <v>3889.409402516725</v>
+        <v>4088.449422597257</v>
       </c>
       <c r="W9">
-        <v>3885.184528486806</v>
+        <v>4103.94636274034</v>
       </c>
       <c r="X9">
-        <v>4117.643147798251</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y9">
-        <v>4086.72813047241</v>
+        <v>4118.3382300992</v>
       </c>
       <c r="Z9">
-        <v>4176.633223453386</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA9">
-        <v>3981.845615351559</v>
+        <v>4054.805089244566</v>
       </c>
       <c r="AB9">
-        <v>3947.81345803351</v>
+        <v>3976.960410242727</v>
       </c>
       <c r="AC9">
-        <v>3899.788819976822</v>
+        <v>4003.267882252596</v>
       </c>
       <c r="AD9">
-        <v>3952.860557561129</v>
+        <v>4062.713382010994</v>
       </c>
       <c r="AE9">
         <v>7</v>
       </c>
       <c r="AF9">
-        <v>129.1973340154305</v>
+        <v>94.8057491802824</v>
       </c>
       <c r="AG9">
-        <v>3977.016504368733</v>
+        <v>4034.646157938223</v>
       </c>
       <c r="AH9">
-        <v>4106.213838384164</v>
+        <v>4129.451907118505</v>
       </c>
       <c r="AI9">
-        <v>3847.819170353303</v>
+        <v>3939.84040875794</v>
       </c>
     </row>
     <row r="10" spans="1:35">
       <c r="A10">
-        <v>3876.504347806812</v>
+        <v>4073.150973979763</v>
       </c>
       <c r="B10">
-        <v>4059.340755360652</v>
+        <v>3961.743297273461</v>
       </c>
       <c r="C10">
-        <v>3975.49186220928</v>
+        <v>4115.721103667424</v>
       </c>
       <c r="D10">
-        <v>3934.271527403107</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E10">
-        <v>4061.944200590551</v>
+        <v>4211.169281233559</v>
       </c>
       <c r="F10">
-        <v>4105.729879787218</v>
+        <v>4076.13586166109</v>
       </c>
       <c r="G10">
-        <v>3830.308731341631</v>
+        <v>3963.054608463689</v>
       </c>
       <c r="H10">
-        <v>4080.148293248155</v>
+        <v>4165.596755217855</v>
       </c>
       <c r="I10">
-        <v>3888.194353691815</v>
+        <v>4011.262884979989</v>
       </c>
       <c r="J10">
-        <v>3872.912727445029</v>
+        <v>3957.067505419134</v>
       </c>
       <c r="K10">
-        <v>4161.364295913424</v>
+        <v>4060.687041401625</v>
       </c>
       <c r="L10">
-        <v>3582.818119354935</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M10">
-        <v>4021.009866910494</v>
+        <v>3857.687076954601</v>
       </c>
       <c r="N10">
-        <v>4036.781481655154</v>
+        <v>3898.995416859769</v>
       </c>
       <c r="O10">
-        <v>3742.104510259517</v>
+        <v>4090.793752666073</v>
       </c>
       <c r="P10">
-        <v>4193.301722847783</v>
+        <v>3987.020649790948</v>
       </c>
       <c r="Q10">
-        <v>4083.539854912701</v>
+        <v>4028.797655952813</v>
       </c>
       <c r="R10">
-        <v>3917.468736119041</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S10">
-        <v>3874.302871801664</v>
+        <v>4207.059823072322</v>
       </c>
       <c r="T10">
-        <v>3707.438063422706</v>
+        <v>3991.189763750467</v>
       </c>
       <c r="U10">
-        <v>4008.77341602358</v>
+        <v>4021.217076499784</v>
       </c>
       <c r="V10">
-        <v>3889.409402516725</v>
+        <v>4088.449422597257</v>
       </c>
       <c r="W10">
-        <v>3885.184528486806</v>
+        <v>4103.94636274034</v>
       </c>
       <c r="X10">
-        <v>4117.643147798251</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y10">
-        <v>4060.675531269419</v>
+        <v>4118.3382300992</v>
       </c>
       <c r="Z10">
-        <v>4176.633223453386</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA10">
-        <v>3981.845615351559</v>
+        <v>4054.805089244566</v>
       </c>
       <c r="AB10">
-        <v>3904.353809646612</v>
+        <v>3976.960410242727</v>
       </c>
       <c r="AC10">
-        <v>3899.788819976822</v>
+        <v>4003.267882252596</v>
       </c>
       <c r="AD10">
-        <v>3952.860557561129</v>
+        <v>4062.713382010994</v>
       </c>
       <c r="AE10">
         <v>8</v>
       </c>
       <c r="AF10">
-        <v>141.1542149771268</v>
+        <v>94.37113947821612</v>
       </c>
       <c r="AG10">
-        <v>3962.738141805532</v>
+        <v>4030.278438218636</v>
       </c>
       <c r="AH10">
-        <v>4103.892356782659</v>
+        <v>4124.649577696852</v>
       </c>
       <c r="AI10">
-        <v>3821.583926828405</v>
+        <v>3935.90729874042</v>
       </c>
     </row>
     <row r="11" spans="1:35">
       <c r="A11">
-        <v>3860.156550534577</v>
+        <v>4073.150973979763</v>
       </c>
       <c r="B11">
-        <v>3888.828635297548</v>
+        <v>3961.743297273461</v>
       </c>
       <c r="C11">
-        <v>3946.290375547124</v>
+        <v>4115.721103667424</v>
       </c>
       <c r="D11">
-        <v>3934.271527403107</v>
+        <v>3879.56857466587</v>
       </c>
       <c r="E11">
-        <v>4061.944200590551</v>
+        <v>4186.956042960988</v>
       </c>
       <c r="F11">
-        <v>4105.729879787218</v>
+        <v>4076.13586166109</v>
       </c>
       <c r="G11">
-        <v>3830.308731341631</v>
+        <v>3963.054608463689</v>
       </c>
       <c r="H11">
-        <v>4080.148293248155</v>
+        <v>4143.277104190689</v>
       </c>
       <c r="I11">
-        <v>3888.194353691815</v>
+        <v>4011.262884979989</v>
       </c>
       <c r="J11">
-        <v>3872.912727445029</v>
+        <v>3951.996943790778</v>
       </c>
       <c r="K11">
-        <v>4161.364295913424</v>
+        <v>4060.687041401625</v>
       </c>
       <c r="L11">
-        <v>3582.818119354935</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M11">
-        <v>4021.009866910494</v>
+        <v>3857.687076954601</v>
       </c>
       <c r="N11">
-        <v>3929.144662485524</v>
+        <v>3898.995416859769</v>
       </c>
       <c r="O11">
-        <v>3742.104510259517</v>
+        <v>4077.085650267751</v>
       </c>
       <c r="P11">
-        <v>4036.53995309705</v>
+        <v>3987.020649790948</v>
       </c>
       <c r="Q11">
-        <v>4023.57917804749</v>
+        <v>3990.044169276255</v>
       </c>
       <c r="R11">
-        <v>3834.185813160205</v>
+        <v>4138.677876738978</v>
       </c>
       <c r="S11">
-        <v>3868.628057416159</v>
+        <v>4207.059823072322</v>
       </c>
       <c r="T11">
-        <v>3707.438063422706</v>
+        <v>3923.511757890763</v>
       </c>
       <c r="U11">
-        <v>4008.77341602358</v>
+        <v>3948.046647506439</v>
       </c>
       <c r="V11">
-        <v>3819.228336323561</v>
+        <v>4023.44003937617</v>
       </c>
       <c r="W11">
-        <v>3885.184528486806</v>
+        <v>3962.874990755126</v>
       </c>
       <c r="X11">
-        <v>4059.245376128709</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y11">
-        <v>3921.761139931309</v>
+        <v>4118.3382300992</v>
       </c>
       <c r="Z11">
-        <v>4176.633223453386</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA11">
-        <v>3981.845615351559</v>
+        <v>4028.796494631081</v>
       </c>
       <c r="AB11">
-        <v>3805.897927000234</v>
+        <v>3976.960410242727</v>
       </c>
       <c r="AC11">
-        <v>3882.811179538926</v>
+        <v>4003.267882252596</v>
       </c>
       <c r="AD11">
-        <v>3952.860557561129</v>
+        <v>4062.713382010994</v>
       </c>
       <c r="AE11">
         <v>9</v>
       </c>
       <c r="AF11">
-        <v>132.8430036262417</v>
+        <v>92.77626235813189</v>
       </c>
       <c r="AG11">
-        <v>3928.994636491782</v>
+        <v>4014.378344062776</v>
       </c>
       <c r="AH11">
-        <v>4061.837640118024</v>
+        <v>4107.154606420908</v>
       </c>
       <c r="AI11">
-        <v>3796.151632865541</v>
+        <v>3921.602081704644</v>
       </c>
     </row>
     <row r="12" spans="1:35">
       <c r="A12">
-        <v>3794.653020043877</v>
+        <v>3950.987610914658</v>
       </c>
       <c r="B12">
-        <v>3888.828635297548</v>
+        <v>3961.743297273461</v>
       </c>
       <c r="C12">
-        <v>3906.852602915739</v>
+        <v>4115.721103667424</v>
       </c>
       <c r="D12">
-        <v>3824.455119146661</v>
+        <v>3845.12188112924</v>
       </c>
       <c r="E12">
-        <v>4061.944200590551</v>
+        <v>4182.224352183007</v>
       </c>
       <c r="F12">
-        <v>4105.729879787218</v>
+        <v>4076.13586166109</v>
       </c>
       <c r="G12">
-        <v>3830.308731341631</v>
+        <v>3963.054608463689</v>
       </c>
       <c r="H12">
-        <v>4080.148293248155</v>
+        <v>4143.277104190689</v>
       </c>
       <c r="I12">
-        <v>3888.194353691815</v>
+        <v>3911.81228068915</v>
       </c>
       <c r="J12">
-        <v>3872.912727445029</v>
+        <v>3951.996943790778</v>
       </c>
       <c r="K12">
-        <v>4161.364295913424</v>
+        <v>4060.687041401625</v>
       </c>
       <c r="L12">
-        <v>3582.818119354935</v>
+        <v>4007.831702098206</v>
       </c>
       <c r="M12">
-        <v>4021.009866910494</v>
+        <v>3857.687076954601</v>
       </c>
       <c r="N12">
-        <v>3929.144662485524</v>
+        <v>3898.995416859769</v>
       </c>
       <c r="O12">
-        <v>3730.524520977293</v>
+        <v>4077.085650267751</v>
       </c>
       <c r="P12">
-        <v>4036.53995309705</v>
+        <v>3987.020649790948</v>
       </c>
       <c r="Q12">
-        <v>4023.57917804749</v>
+        <v>3914.009587290188</v>
       </c>
       <c r="R12">
-        <v>3815.950759670592</v>
+        <v>3990.491208149441</v>
       </c>
       <c r="S12">
-        <v>3857.224278352653</v>
+        <v>4137.92762472397</v>
       </c>
       <c r="T12">
-        <v>3659.841069047226</v>
+        <v>3923.511757890763</v>
       </c>
       <c r="U12">
-        <v>4008.77341602358</v>
+        <v>3933.02389931131</v>
       </c>
       <c r="V12">
-        <v>3767.663951912773</v>
+        <v>4023.44003937617</v>
       </c>
       <c r="W12">
-        <v>3885.184528486806</v>
+        <v>3900.476813571693</v>
       </c>
       <c r="X12">
-        <v>4059.245376128709</v>
+        <v>3935.228258331817</v>
       </c>
       <c r="Y12">
-        <v>3915.688793922054</v>
+        <v>4027.95152112983</v>
       </c>
       <c r="Z12">
-        <v>3875.242430188273</v>
+        <v>3860.215426692186</v>
       </c>
       <c r="AA12">
-        <v>3981.845615351559</v>
+        <v>3939.258368445906</v>
       </c>
       <c r="AB12">
-        <v>3805.897927000234</v>
+        <v>3976.960410242727</v>
       </c>
       <c r="AC12">
-        <v>3882.811179538926</v>
+        <v>4003.267882252596</v>
       </c>
       <c r="AD12">
-        <v>3952.860557561129</v>
+        <v>4018.032546330099</v>
       </c>
       <c r="AE12">
         <v>10</v>
       </c>
       <c r="AF12">
-        <v>132.6546871730062</v>
+        <v>87.6685394739895</v>
       </c>
       <c r="AG12">
-        <v>3906.907934782631</v>
+        <v>3985.83926416916</v>
       </c>
       <c r="AH12">
-        <v>4039.562621955637</v>
+        <v>4073.507803643149</v>
       </c>
       <c r="AI12">
-        <v>3774.253247609625</v>
+        <v>3898.170724695171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>